<commit_message>
bug fix and deprecated code deletion.
</commit_message>
<xml_diff>
--- a/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
+++ b/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/118932b6e8a6f92f/ETHY3FW/semesterProjectYiqiaoWang/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangy\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1302" documentId="8_{B7C037C4-79D8-4A18-8425-09F0EAB31306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FECA15F-3693-4944-AAA2-8EA3454982A2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE596B14-061C-4FD1-BF76-D849F30C747F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15943" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
+    <workbookView xWindow="-22046" yWindow="8649" windowWidth="22149" windowHeight="13200" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
   </bookViews>
   <sheets>
     <sheet name="supply" sheetId="5" r:id="rId1"/>
@@ -663,6 +663,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{58ABB07C-8821-40E3-8620-1B9FF3CEFAEF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+just a placeholder for now.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -911,7 +935,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-outside temeprature -5</t>
+here, ASHP cannot work reversely and create cooling. Addition chiller should be added to the system.</t>
         </r>
       </text>
     </comment>
@@ -2017,7 +2041,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="122">
   <si>
     <t>monetary</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2486,6 +2510,10 @@
   </si>
   <si>
     <t>carrier_ratios</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PVT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2571,7 +2599,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2584,12 +2612,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -2597,6 +2619,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2953,50 +2978,50 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.35546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.92578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.92578125" customWidth="1"/>
-    <col min="7" max="7" width="7.78515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.9140625" customWidth="1"/>
+    <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="7"/>
       <c r="G2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="4"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
@@ -3025,237 +3050,237 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="5" t="s">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4">
         <v>0.05</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4">
         <v>2.4E-2</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="5" t="s">
+      <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" t="s">
         <v>107</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5">
         <v>0.05</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5">
         <v>1.6E-2</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="5" t="s">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6">
         <v>0.05</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="5" t="s">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7">
         <v>0.13250000000000001</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7">
         <v>0.05</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7">
         <v>0.23</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8">
         <v>0.14299999999999999</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8">
         <v>0.05</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8">
         <f>AVERAGE(G7,G9)</f>
         <v>0.17699999999999999</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="5" t="s">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9">
         <v>0.17799999999999999</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9">
         <v>0.05</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9">
         <v>0.124</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="5" t="s">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" t="s">
         <v>107</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10">
         <v>0.10199999999999999</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10">
         <v>0.05</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10">
         <v>2.8000000000000001E-2</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="5" t="s">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11">
         <v>0.1</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11">
         <v>0.05</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11">
         <v>0.32400000000000001</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" t="s">
         <v>107</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12">
         <v>0.122</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12">
         <v>0.05</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12">
         <v>1</v>
       </c>
     </row>
@@ -3274,71 +3299,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561E90E2-20B4-48EB-B5A5-7E82D5B88F8D}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="12.92578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.35546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.78515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.78515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.0703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.2109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.0703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.08203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.08203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
@@ -3628,6 +3653,20 @@
       </c>
       <c r="N9">
         <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F10">
+        <v>0.05</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3648,68 +3687,68 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G31" sqref="A1:XFD1048576"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.78515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.35546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.78515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.0703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.0703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.08203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">
@@ -4678,133 +4717,133 @@
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView zoomScale="77" workbookViewId="0">
-      <selection activeCell="G43" sqref="A1:XFD1048576"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.35546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.2109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.2109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.78515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.2109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="7.78515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.2109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.0703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.08203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
       <c r="N2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
     </row>
     <row r="3" spans="1:21">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="7" t="s">
         <v>28</v>
       </c>
       <c r="P3" s="8" t="s">
@@ -4812,71 +4851,71 @@
       </c>
       <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="4" t="s">
+      <c r="U3" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
       <c r="P4" s="8" t="s">
         <v>101</v>
       </c>
       <c r="Q4" s="8"/>
-      <c r="R4" s="9" t="s">
+      <c r="R4" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="7" t="s">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="R5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
@@ -4915,9 +4954,9 @@
       <c r="O6">
         <v>0.55000000000000004</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6">
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4">
         <v>0.64</v>
       </c>
       <c r="S6">
@@ -4961,11 +5000,11 @@
       <c r="O7">
         <v>8</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="4">
         <f>O7-1</f>
         <v>7</v>
       </c>
-      <c r="R7" s="6"/>
+      <c r="R7" s="4"/>
       <c r="S7">
         <v>5</v>
       </c>
@@ -5007,11 +5046,11 @@
       <c r="O8">
         <v>4.4400000000000004</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="4">
         <f>O8-1</f>
         <v>3.4400000000000004</v>
       </c>
-      <c r="R8" s="6"/>
+      <c r="R8" s="4"/>
       <c r="S8">
         <v>5</v>
       </c>
@@ -5053,8 +5092,8 @@
       <c r="O9">
         <v>8</v>
       </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6">
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4">
         <f>O9-1</f>
         <v>7</v>
       </c>
@@ -5070,14 +5109,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="T3:T5"/>
-    <mergeCell ref="U3:U5"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="E3:E5"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="S3:S5"/>
     <mergeCell ref="N3:N5"/>
@@ -5094,6 +5125,14 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="O3:O5"/>
+    <mergeCell ref="T3:T5"/>
+    <mergeCell ref="U3:U5"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="E3:E5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5109,65 +5148,65 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="11.78515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.0703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.08203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.78515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.0703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.08203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="3" t="s">

</xml_diff>

<commit_message>
update the energy hub functions to fit the current technology definition file
</commit_message>
<xml_diff>
--- a/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
+++ b/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangy\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE596B14-061C-4FD1-BF76-D849F30C747F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D79700-A920-4E4C-9176-8892926E2011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22046" yWindow="8649" windowWidth="22149" windowHeight="13200" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
   </bookViews>
   <sheets>
     <sheet name="supply" sheetId="5" r:id="rId1"/>
@@ -298,7 +298,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{381592D0-4B82-44EA-8DB3-F97383AB5D21}">
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{381592D0-4B82-44EA-8DB3-F97383AB5D21}">
       <text>
         <r>
           <rPr>
@@ -322,7 +322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{61312002-E024-4292-93F4-FD63A14A1DFD}">
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{61312002-E024-4292-93F4-FD63A14A1DFD}">
       <text>
         <r>
           <rPr>
@@ -347,7 +347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{A439E244-A83C-403E-BC74-150106BD9060}">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{A439E244-A83C-403E-BC74-150106BD9060}">
       <text>
         <r>
           <rPr>
@@ -371,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{F156C5E5-9988-454F-B199-E54895C12234}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{F156C5E5-9988-454F-B199-E54895C12234}">
       <text>
         <r>
           <rPr>
@@ -395,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{AEFC007F-1ADD-4627-B6DF-D92185D067E3}">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{AEFC007F-1ADD-4627-B6DF-D92185D067E3}">
       <text>
         <r>
           <rPr>
@@ -419,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{164D751A-85F8-4A50-833D-EAAD0DAA59C2}">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{164D751A-85F8-4A50-833D-EAAD0DAA59C2}">
       <text>
         <r>
           <rPr>
@@ -543,7 +543,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{DD74A52F-1054-45EF-9073-B14456474A5B}">
+    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{DD74A52F-1054-45EF-9073-B14456474A5B}">
       <text>
         <r>
           <rPr>
@@ -567,7 +567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{2DCFA103-1274-4847-83A7-AC3F88F17291}">
+    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{2DCFA103-1274-4847-83A7-AC3F88F17291}">
       <text>
         <r>
           <rPr>
@@ -615,7 +615,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{BF918F83-D58B-46AA-AB83-02772C77D60C}">
+    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{BF918F83-D58B-46AA-AB83-02772C77D60C}">
       <text>
         <r>
           <rPr>
@@ -639,7 +639,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{960AF645-C149-407D-B0B9-2EF4831D05BD}">
+    <comment ref="O9" authorId="0" shapeId="0" xr:uid="{960AF645-C149-407D-B0B9-2EF4831D05BD}">
       <text>
         <r>
           <rPr>
@@ -771,7 +771,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{34B10223-7A34-446D-BC14-3CEB6051B6A9}">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{34B10223-7A34-446D-BC14-3CEB6051B6A9}">
       <text>
         <r>
           <rPr>
@@ -795,7 +795,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{F68FE046-B4A1-4E11-A3F9-22AEA125C71A}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{F68FE046-B4A1-4E11-A3F9-22AEA125C71A}">
       <text>
         <r>
           <rPr>
@@ -819,7 +819,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{2A5008E0-6771-496C-A929-12D90B68E371}">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{2A5008E0-6771-496C-A929-12D90B68E371}">
       <text>
         <r>
           <rPr>
@@ -843,7 +843,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{2E9194AA-01A3-4783-B5CF-A05FF31A6CD7}">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{2E9194AA-01A3-4783-B5CF-A05FF31A6CD7}">
       <text>
         <r>
           <rPr>
@@ -987,7 +987,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{8D30FF0A-F524-4BAB-A2A9-55CA0982EF14}">
+    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{8D30FF0A-F524-4BAB-A2A9-55CA0982EF14}">
       <text>
         <r>
           <rPr>
@@ -1012,7 +1012,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{21E87ED6-F24A-4DA0-A3F6-1520504A752B}">
+    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{21E87ED6-F24A-4DA0-A3F6-1520504A752B}">
       <text>
         <r>
           <rPr>
@@ -1036,7 +1036,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{0E42BBB0-E2D2-4B44-A8FB-B6C155C3EBB8}">
+    <comment ref="L9" authorId="0" shapeId="0" xr:uid="{0E42BBB0-E2D2-4B44-A8FB-B6C155C3EBB8}">
       <text>
         <r>
           <rPr>
@@ -1108,7 +1108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N10" authorId="0" shapeId="0" xr:uid="{F03E95D3-22AC-4F5A-A01A-E49103ED38DC}">
+    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{F03E95D3-22AC-4F5A-A01A-E49103ED38DC}">
       <text>
         <r>
           <rPr>
@@ -1180,7 +1180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N12" authorId="0" shapeId="0" xr:uid="{0C0424B8-830D-41AF-9090-E6C9C5134069}">
+    <comment ref="O12" authorId="0" shapeId="0" xr:uid="{0C0424B8-830D-41AF-9090-E6C9C5134069}">
       <text>
         <r>
           <rPr>
@@ -1372,7 +1372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N23" authorId="0" shapeId="0" xr:uid="{AF2745AD-0BD1-40F0-B7C8-39776BC84E0B}">
+    <comment ref="O23" authorId="0" shapeId="0" xr:uid="{AF2745AD-0BD1-40F0-B7C8-39776BC84E0B}">
       <text>
         <r>
           <rPr>
@@ -1481,7 +1481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{7F409247-01A7-4BC4-AF03-5B83C1D294AC}">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{7F409247-01A7-4BC4-AF03-5B83C1D294AC}">
       <text>
         <r>
           <rPr>
@@ -1505,7 +1505,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{E073AC29-9FBC-4783-A1CC-EAB82E58C39C}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{E073AC29-9FBC-4783-A1CC-EAB82E58C39C}">
       <text>
         <r>
           <rPr>
@@ -1529,7 +1529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{172F2BCC-F594-42BB-94FD-9D042C47C8B7}">
+    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{172F2BCC-F594-42BB-94FD-9D042C47C8B7}">
       <text>
         <r>
           <rPr>
@@ -1553,7 +1553,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{17EE350A-94DF-4B20-A644-8F0113B68800}">
+    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{17EE350A-94DF-4B20-A644-8F0113B68800}">
       <text>
         <r>
           <rPr>
@@ -1577,7 +1577,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{641BB6AA-8D9F-47C1-B8F2-8D68B1629C5D}">
+    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{641BB6AA-8D9F-47C1-B8F2-8D68B1629C5D}">
       <text>
         <r>
           <rPr>
@@ -1601,7 +1601,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P5" authorId="0" shapeId="0" xr:uid="{6E37FAD6-A059-45C2-A830-57EB8A2A5A6C}">
+    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{6E37FAD6-A059-45C2-A830-57EB8A2A5A6C}">
       <text>
         <r>
           <rPr>
@@ -1625,7 +1625,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{2A99EE64-0296-41DD-93CB-4EFDCB3E6708}">
+    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{2A99EE64-0296-41DD-93CB-4EFDCB3E6708}">
       <text>
         <r>
           <rPr>
@@ -1653,7 +1653,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U6" authorId="1" shapeId="0" xr:uid="{4BB9E1A7-B022-46AE-9E98-BC8F14DC2BFC}">
+    <comment ref="V6" authorId="1" shapeId="0" xr:uid="{4BB9E1A7-B022-46AE-9E98-BC8F14DC2BFC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1661,7 +1661,7 @@
     from ChatGPT, need revision</t>
       </text>
     </comment>
-    <comment ref="O7" authorId="0" shapeId="0" xr:uid="{70D642DE-32B4-422D-B900-B8F154C15536}">
+    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{70D642DE-32B4-422D-B900-B8F154C15536}">
       <text>
         <r>
           <rPr>
@@ -1689,7 +1689,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{EEF463E6-46EB-4F38-A33E-3A2E4076E8BB}">
+    <comment ref="Q7" authorId="0" shapeId="0" xr:uid="{EEF463E6-46EB-4F38-A33E-3A2E4076E8BB}">
       <text>
         <r>
           <rPr>
@@ -1748,7 +1748,79 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{AD232550-4ED0-422A-8658-387310324587}">
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{3B3036DA-5E93-4550-A99C-8E9D560CBC20}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+annual o&amp;m cost relative to the investment cost [1]</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{838C1899-AD71-407A-892C-57CED5C28137}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+charging/discharging efficiency of conversion technology. Note: the round trip efficiency would be the square of this value!</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{F0749ECF-8748-463A-AB60-85E38149A943}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+[kW], maximum technology installation capacity</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{227B468A-D31B-4B26-AB25-82ACAC0160B1}">
       <text>
         <r>
           <rPr>
@@ -1772,79 +1844,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{3B3036DA-5E93-4550-A99C-8E9D560CBC20}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-annual o&amp;m cost relative to the investment cost [1]</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{838C1899-AD71-407A-892C-57CED5C28137}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-charging/discharging efficiency of conversion technology. Note: the round trip efficiency would be the square of this value!</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{F0749ECF-8748-463A-AB60-85E38149A943}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-[kW], maximum technology installation capacity</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{6B04D491-22C5-4C9D-8E0F-C5484E44DCCD}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{6B04D491-22C5-4C9D-8E0F-C5484E44DCCD}">
       <text>
         <r>
           <rPr>
@@ -1868,7 +1868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{FC9B2166-9A6E-4D98-AD30-E36CE6C3D758}">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{FC9B2166-9A6E-4D98-AD30-E36CE6C3D758}">
       <text>
         <r>
           <rPr>
@@ -1916,7 +1916,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{D6700C79-ABD9-4561-AF6A-4D6F81765EEA}">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{D6700C79-ABD9-4561-AF6A-4D6F81765EEA}">
       <text>
         <r>
           <rPr>
@@ -1988,7 +1988,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{1A6C0AA1-F43C-4456-8725-7879AC904B28}">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{1A6C0AA1-F43C-4456-8725-7879AC904B28}">
       <text>
         <r>
           <rPr>
@@ -2012,7 +2012,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{B7E1B3AF-3A44-4383-BFA8-257E2C687078}">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{B7E1B3AF-3A44-4383-BFA8-257E2C687078}">
       <text>
         <r>
           <rPr>
@@ -2041,7 +2041,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="123">
   <si>
     <t>monetary</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2514,6 +2514,10 @@
   </si>
   <si>
     <t>PVT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>placeholder</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2967,7 +2971,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="U6" dT="2024-10-16T23:38:04.56" personId="{BAD9BABF-23D2-4A7A-A5F9-262A050E563D}" id="{4BB9E1A7-B022-46AE-9E98-BC8F14DC2BFC}">
+  <threadedComment ref="V6" dT="2024-10-16T23:38:04.56" personId="{BAD9BABF-23D2-4A7A-A5F9-262A050E563D}" id="{4BB9E1A7-B022-46AE-9E98-BC8F14DC2BFC}">
     <text>from ChatGPT, need revision</text>
   </threadedComment>
 </ThreadedComments>
@@ -2977,7 +2981,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2603C43B-861B-457A-A24B-3EBFF53534AD}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -3299,10 +3303,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561E90E2-20B4-48EB-B5A5-7E82D5B88F8D}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -3315,15 +3319,16 @@
     <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.08203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.08203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.08203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -3336,16 +3341,17 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3355,7 +3361,7 @@
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="I2" s="7"/>
@@ -3364,8 +3370,9 @@
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -3391,25 +3398,28 @@
         <v>22</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3428,32 +3438,29 @@
       <c r="F4">
         <v>0.05</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
       <c r="H4">
         <v>1250</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
         <v>89</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>5.56</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>42</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
+      <c r="N4">
         <v>10</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3478,26 +3485,29 @@
       <c r="H5">
         <v>1250</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
         <v>89</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>5.56</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>42</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>10</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>100</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3522,26 +3532,29 @@
       <c r="H6">
         <v>1250</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
         <v>89</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>5.56</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>42</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>100</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>200</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3560,32 +3573,29 @@
       <c r="F7">
         <v>0.05</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
       <c r="H7">
         <v>1250</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
         <v>89</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>5.56</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>42</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>200</v>
       </c>
-      <c r="M7">
-        <v>1000</v>
-      </c>
-      <c r="N7">
+      <c r="O7">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -3604,23 +3614,23 @@
       <c r="F8">
         <v>0.05</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
       <c r="H8">
         <v>290</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
         <v>89</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>2</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -3639,42 +3649,46 @@
       <c r="F9">
         <v>0.05</v>
       </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
       <c r="H9">
         <v>296</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
         <v>89</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>1.7</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>121</v>
       </c>
       <c r="C10" t="s">
         <v>107</v>
       </c>
+      <c r="D10" t="s">
+        <v>122</v>
+      </c>
       <c r="F10">
         <v>0.05</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:N2"/>
+    <mergeCell ref="J1:O2"/>
     <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3684,10 +3698,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A246388-C9BA-4771-92A8-398DB13C28C5}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -3702,13 +3716,14 @@
     <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.58203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.08203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.08203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -3723,14 +3738,15 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="7"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3742,15 +3758,16 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -3782,19 +3799,22 @@
         <v>22</v>
       </c>
       <c r="K3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -3826,19 +3846,22 @@
         <v>4.7709999999999999</v>
       </c>
       <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
         <v>0.95</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>15</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>50</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -3870,19 +3893,22 @@
         <v>4.7709999999999999</v>
       </c>
       <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
         <v>0.95</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>50</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>200</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -3914,19 +3940,22 @@
         <v>4.7709999999999999</v>
       </c>
       <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
         <v>0.95</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>200</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>500</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -3958,19 +3987,22 @@
         <v>4.7709999999999999</v>
       </c>
       <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>0.95</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>500</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>2000</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -4002,19 +4034,22 @@
         <v>45.9</v>
       </c>
       <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
         <v>4.58</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>1</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>200</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -4046,19 +4081,22 @@
         <v>36.299999999999997</v>
       </c>
       <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
         <v>5.45</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>5</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>1000</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -4090,19 +4128,22 @@
         <v>45.9</v>
       </c>
       <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
         <v>2.89</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>1</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>200</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -4134,19 +4175,22 @@
         <v>36.299999999999997</v>
       </c>
       <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
         <v>3.44</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>5</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>1000</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -4178,19 +4222,22 @@
         <v>45.9</v>
       </c>
       <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
         <v>2.2000000000000002</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>1</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>200</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -4222,19 +4269,22 @@
         <v>36.299999999999997</v>
       </c>
       <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <v>2.6</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>5</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>1000</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -4266,19 +4316,22 @@
         <v>37.685000000000002</v>
       </c>
       <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
         <v>0.91</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>1</v>
-      </c>
-      <c r="M14">
-        <v>20</v>
       </c>
       <c r="N14">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="O14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -4310,19 +4363,22 @@
         <v>77.900000000000006</v>
       </c>
       <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
         <v>0.89</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>1</v>
-      </c>
-      <c r="M15">
-        <v>20</v>
       </c>
       <c r="N15">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="O15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -4354,19 +4410,22 @@
         <v>44.555</v>
       </c>
       <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
         <v>0.92</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>1</v>
-      </c>
-      <c r="M16">
-        <v>20</v>
       </c>
       <c r="N16">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>51</v>
       </c>
@@ -4398,19 +4457,22 @@
         <v>18.100000000000001</v>
       </c>
       <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
         <v>0.91</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>20</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <v>200</v>
       </c>
-      <c r="N17">
+      <c r="O17">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -4442,19 +4504,22 @@
         <v>19.399999999999999</v>
       </c>
       <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <v>0.89</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>20</v>
       </c>
-      <c r="M18">
+      <c r="N18">
         <v>200</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -4486,19 +4551,22 @@
         <v>25.07</v>
       </c>
       <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
         <v>0.92</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>20</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <v>200</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -4530,19 +4598,22 @@
         <v>18.100000000000001</v>
       </c>
       <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
         <v>0.91</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>200</v>
       </c>
-      <c r="M20">
+      <c r="N20">
         <v>500</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -4574,19 +4645,22 @@
         <v>19.399999999999999</v>
       </c>
       <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
         <v>0.89</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>200</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>500</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -4618,19 +4692,22 @@
         <v>19.510000000000002</v>
       </c>
       <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
         <v>0.92</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>200</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>500</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -4647,13 +4724,16 @@
         <v>0.05</v>
       </c>
       <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
         <v>1</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -4670,13 +4750,16 @@
         <v>0.05</v>
       </c>
       <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
         <v>1</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -4693,18 +4776,22 @@
         <v>0.05</v>
       </c>
       <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
         <v>1</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="F2:I2"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N2"/>
+    <mergeCell ref="L1:O2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="F1:K1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4714,10 +4801,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CCA624-D427-4AF6-862A-48646A94FFF1}">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -4735,16 +4822,17 @@
     <col min="11" max="11" width="11.75" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.08203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.58203125" customWidth="1"/>
+    <col min="16" max="16" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -4763,17 +4851,18 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="7"/>
+      <c r="P1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
       <c r="R1" s="7"/>
       <c r="S1" s="7"/>
       <c r="T1" s="7"/>
       <c r="U1" s="7"/>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="V1" s="7"/>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -4789,7 +4878,7 @@
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="7" t="s">
         <v>26</v>
       </c>
       <c r="O2" s="7"/>
@@ -4799,8 +4888,9 @@
       <c r="S2" s="7"/>
       <c r="T2" s="7"/>
       <c r="U2" s="7"/>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="V2" s="7"/>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" s="7" t="s">
         <v>32</v>
       </c>
@@ -4841,27 +4931,30 @@
         <v>23</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O3" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="Q3" s="8"/>
       <c r="R3" s="8"/>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="8"/>
+      <c r="T3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="U3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="V3" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -4877,18 +4970,19 @@
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="7"/>
+      <c r="Q4" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="6" t="s">
+      <c r="R4" s="8"/>
+      <c r="S4" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="S4" s="7"/>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="V4" s="7"/>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -4904,20 +4998,21 @@
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="7"/>
+      <c r="Q5" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" s="5" t="s">
+      <c r="R5" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="R5" s="5" t="s">
+      <c r="S5" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="V5" s="7"/>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>100</v>
       </c>
@@ -4952,24 +5047,27 @@
         <v>86.82</v>
       </c>
       <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
         <v>0.55000000000000004</v>
       </c>
-      <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="4">
+      <c r="R6" s="4"/>
+      <c r="S6" s="4">
         <v>0.64</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>10</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>500</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>117</v>
       </c>
@@ -4997,25 +5095,34 @@
       <c r="L7">
         <v>55600</v>
       </c>
+      <c r="M7">
+        <v>11.57</v>
+      </c>
+      <c r="N7">
+        <v>36.299999999999997</v>
+      </c>
       <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
         <v>8</v>
       </c>
-      <c r="P7" s="4">
-        <f>O7-1</f>
+      <c r="Q7" s="4">
+        <f>P7-1</f>
         <v>7</v>
       </c>
-      <c r="R7" s="4"/>
-      <c r="S7">
+      <c r="S7" s="4"/>
+      <c r="T7">
         <v>5</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>500</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -5043,25 +5150,34 @@
       <c r="L8">
         <v>55600</v>
       </c>
+      <c r="M8">
+        <v>11.57</v>
+      </c>
+      <c r="N8">
+        <v>36.299999999999997</v>
+      </c>
       <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
         <v>4.4400000000000004</v>
       </c>
-      <c r="P8" s="4">
-        <f>O8-1</f>
+      <c r="Q8" s="4">
+        <f>P8-1</f>
         <v>3.4400000000000004</v>
       </c>
-      <c r="R8" s="4"/>
-      <c r="S8">
+      <c r="S8" s="4"/>
+      <c r="T8">
         <v>5</v>
       </c>
-      <c r="T8">
+      <c r="U8">
         <v>500</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>119</v>
       </c>
@@ -5089,50 +5205,61 @@
       <c r="L9">
         <v>55600</v>
       </c>
+      <c r="M9">
+        <v>11.57</v>
+      </c>
+      <c r="N9">
+        <v>36.299999999999997</v>
+      </c>
       <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
         <v>8</v>
       </c>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4">
-        <f>O9-1</f>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4">
+        <f>P9-1</f>
         <v>7</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>5</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>500</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="26">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="P3:P5"/>
+    <mergeCell ref="U3:U5"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="J1:O1"/>
     <mergeCell ref="D3:D5"/>
-    <mergeCell ref="S3:S5"/>
+    <mergeCell ref="T3:T5"/>
     <mergeCell ref="N3:N5"/>
     <mergeCell ref="M3:M5"/>
     <mergeCell ref="L3:L5"/>
     <mergeCell ref="K3:K5"/>
     <mergeCell ref="J3:J5"/>
     <mergeCell ref="H3:H5"/>
-    <mergeCell ref="J1:N1"/>
-    <mergeCell ref="O1:U2"/>
+    <mergeCell ref="O3:O5"/>
+    <mergeCell ref="P1:V2"/>
     <mergeCell ref="J2:M2"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="O3:O5"/>
-    <mergeCell ref="T3:T5"/>
-    <mergeCell ref="U3:U5"/>
-    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="V3:V5"/>
     <mergeCell ref="A1:I2"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="E3:E5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5142,10 +5269,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED8072C-161B-4E9B-9246-F2F0563C6573}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="14"/>
@@ -5155,18 +5282,19 @@
     <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.4140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.08203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.4140625" customWidth="1"/>
     <col min="10" max="10" width="10.08203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -5187,8 +5315,9 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" s="7"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -5198,17 +5327,18 @@
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -5225,16 +5355,16 @@
         <v>82</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>28</v>
@@ -5243,16 +5373,19 @@
         <v>30</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>57</v>
       </c>
@@ -5269,16 +5402,16 @@
         <v>367</v>
       </c>
       <c r="F4">
-        <v>0.25</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="G4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H4">
-        <v>0.05</v>
+        <v>241.5</v>
       </c>
       <c r="I4">
-        <v>241.5</v>
+        <v>0</v>
       </c>
       <c r="J4">
         <v>0.91</v>
@@ -5287,16 +5420,19 @@
         <v>1000</v>
       </c>
       <c r="L4">
+        <v>0.25</v>
+      </c>
+      <c r="M4">
         <v>1E-3</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0.5</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -5312,14 +5448,17 @@
       <c r="E5">
         <v>13</v>
       </c>
+      <c r="F5">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="G5">
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H5">
-        <v>0.05</v>
+        <v>7</v>
       </c>
       <c r="I5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0.96</v>
@@ -5327,17 +5466,17 @@
       <c r="K5">
         <v>1000</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>0.01</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>0.5</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -5353,14 +5492,17 @@
       <c r="E6">
         <v>13</v>
       </c>
+      <c r="F6">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="G6">
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H6">
-        <v>0.05</v>
+        <v>7</v>
       </c>
       <c r="I6">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J6">
         <v>0.96</v>
@@ -5368,17 +5510,17 @@
       <c r="K6">
         <v>1000</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>0.5</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>81</v>
       </c>
@@ -5394,14 +5536,17 @@
       <c r="E7">
         <v>13</v>
       </c>
+      <c r="F7">
+        <v>1.4999999999999999E-2</v>
+      </c>
       <c r="G7">
-        <v>1.4999999999999999E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H7">
-        <v>0.05</v>
+        <v>7</v>
       </c>
       <c r="I7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0.96</v>
@@ -5409,22 +5554,23 @@
       <c r="K7">
         <v>1000</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>0.02</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>0.5</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>23</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:D2"/>
+    <mergeCell ref="J1:O2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="E1:I1"/>
-    <mergeCell ref="J1:N2"/>
-    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
optimization runs correctly; however the correct implementation of demand technology filtering (as well as emission temperature selection) need to be done (see TODO in district.py)
</commit_message>
<xml_diff>
--- a/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
+++ b/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangy\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D79700-A920-4E4C-9176-8892926E2011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D88AF50-DF68-49F7-9D92-E44A1CFE75DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
+    <workbookView xWindow="-22046" yWindow="8649" windowWidth="22149" windowHeight="13200" activeTab="2" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
   </bookViews>
   <sheets>
     <sheet name="supply" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="conversion" sheetId="6" r:id="rId3"/>
     <sheet name="conversion_plus" sheetId="10" r:id="rId4"/>
     <sheet name="storage" sheetId="8" r:id="rId5"/>
+    <sheet name="demand" sheetId="11" r:id="rId6"/>
+    <sheet name="transmission" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{BF94E0D0-CF1A-4E6A-826E-30BA18B65D8A}">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{BF94E0D0-CF1A-4E6A-826E-30BA18B65D8A}">
       <text>
         <r>
           <rPr>
@@ -273,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{6B6D44A3-5358-49C7-80BA-65B88BAD82BD}">
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{6B6D44A3-5358-49C7-80BA-65B88BAD82BD}">
       <text>
         <r>
           <rPr>
@@ -298,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{381592D0-4B82-44EA-8DB3-F97383AB5D21}">
+    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{381592D0-4B82-44EA-8DB3-F97383AB5D21}">
       <text>
         <r>
           <rPr>
@@ -322,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{61312002-E024-4292-93F4-FD63A14A1DFD}">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{61312002-E024-4292-93F4-FD63A14A1DFD}">
       <text>
         <r>
           <rPr>
@@ -347,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{A439E244-A83C-403E-BC74-150106BD9060}">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{A439E244-A83C-403E-BC74-150106BD9060}">
       <text>
         <r>
           <rPr>
@@ -371,7 +373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{F156C5E5-9988-454F-B199-E54895C12234}">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{F156C5E5-9988-454F-B199-E54895C12234}">
       <text>
         <r>
           <rPr>
@@ -395,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{AEFC007F-1ADD-4627-B6DF-D92185D067E3}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{AEFC007F-1ADD-4627-B6DF-D92185D067E3}">
       <text>
         <r>
           <rPr>
@@ -419,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{164D751A-85F8-4A50-833D-EAAD0DAA59C2}">
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{164D751A-85F8-4A50-833D-EAAD0DAA59C2}">
       <text>
         <r>
           <rPr>
@@ -467,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{637B0CCF-82B9-4C6D-A8BB-FCB6633100EF}">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{637B0CCF-82B9-4C6D-A8BB-FCB6633100EF}">
       <text>
         <r>
           <rPr>
@@ -519,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{F8D9F75B-0547-4549-8288-A925727BEEAA}">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{F8D9F75B-0547-4549-8288-A925727BEEAA}">
       <text>
         <r>
           <rPr>
@@ -543,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{DD74A52F-1054-45EF-9073-B14456474A5B}">
+    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{DD74A52F-1054-45EF-9073-B14456474A5B}">
       <text>
         <r>
           <rPr>
@@ -567,7 +569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{2DCFA103-1274-4847-83A7-AC3F88F17291}">
+    <comment ref="R8" authorId="0" shapeId="0" xr:uid="{2DCFA103-1274-4847-83A7-AC3F88F17291}">
       <text>
         <r>
           <rPr>
@@ -591,7 +593,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{27610EE9-A3A8-40CA-8A0D-BE26099C4505}">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{27610EE9-A3A8-40CA-8A0D-BE26099C4505}">
       <text>
         <r>
           <rPr>
@@ -615,7 +617,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{BF918F83-D58B-46AA-AB83-02772C77D60C}">
+    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{BF918F83-D58B-46AA-AB83-02772C77D60C}">
       <text>
         <r>
           <rPr>
@@ -639,7 +641,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O9" authorId="0" shapeId="0" xr:uid="{960AF645-C149-407D-B0B9-2EF4831D05BD}">
+    <comment ref="R9" authorId="0" shapeId="0" xr:uid="{960AF645-C149-407D-B0B9-2EF4831D05BD}">
       <text>
         <r>
           <rPr>
@@ -1056,7 +1058,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-carnot efficiency 62%, Danish</t>
+carnot efficiency 62%, Danish
+35degC high temp, 10degC low temp (in the ground)</t>
         </r>
       </text>
     </comment>
@@ -1129,6 +1132,30 @@
           </rPr>
           <t xml:space="preserve">
 16-20, Danish energy agency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{C5D0AF4C-BF2F-4C21-9650-2E8E580F6C8C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+60/10</t>
         </r>
       </text>
     </comment>
@@ -1432,7 +1459,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{41DC5FC1-E887-45D5-94A9-4C798351AA4A}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{41DC5FC1-E887-45D5-94A9-4C798351AA4A}">
       <text>
         <r>
           <rPr>
@@ -1457,7 +1484,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{5307FB4B-F2C5-413A-97E2-5B25AE9AA7DC}">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{5307FB4B-F2C5-413A-97E2-5B25AE9AA7DC}">
       <text>
         <r>
           <rPr>
@@ -1481,7 +1508,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{7F409247-01A7-4BC4-AF03-5B83C1D294AC}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{7F409247-01A7-4BC4-AF03-5B83C1D294AC}">
       <text>
         <r>
           <rPr>
@@ -1505,7 +1532,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{E073AC29-9FBC-4783-A1CC-EAB82E58C39C}">
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{E073AC29-9FBC-4783-A1CC-EAB82E58C39C}">
       <text>
         <r>
           <rPr>
@@ -1529,7 +1556,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{172F2BCC-F594-42BB-94FD-9D042C47C8B7}">
+    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{172F2BCC-F594-42BB-94FD-9D042C47C8B7}">
       <text>
         <r>
           <rPr>
@@ -1553,7 +1580,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="0" shapeId="0" xr:uid="{17EE350A-94DF-4B20-A644-8F0113B68800}">
+    <comment ref="W3" authorId="0" shapeId="0" xr:uid="{17EE350A-94DF-4B20-A644-8F0113B68800}">
       <text>
         <r>
           <rPr>
@@ -1577,7 +1604,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="0" shapeId="0" xr:uid="{641BB6AA-8D9F-47C1-B8F2-8D68B1629C5D}">
+    <comment ref="X3" authorId="0" shapeId="0" xr:uid="{641BB6AA-8D9F-47C1-B8F2-8D68B1629C5D}">
       <text>
         <r>
           <rPr>
@@ -1601,7 +1628,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q5" authorId="0" shapeId="0" xr:uid="{6E37FAD6-A059-45C2-A830-57EB8A2A5A6C}">
+    <comment ref="R5" authorId="0" shapeId="0" xr:uid="{6E37FAD6-A059-45C2-A830-57EB8A2A5A6C}">
       <text>
         <r>
           <rPr>
@@ -1625,7 +1652,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S5" authorId="0" shapeId="0" xr:uid="{2A99EE64-0296-41DD-93CB-4EFDCB3E6708}">
+    <comment ref="T5" authorId="0" shapeId="0" xr:uid="{2A99EE64-0296-41DD-93CB-4EFDCB3E6708}">
       <text>
         <r>
           <rPr>
@@ -1653,7 +1680,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V6" authorId="1" shapeId="0" xr:uid="{4BB9E1A7-B022-46AE-9E98-BC8F14DC2BFC}">
+    <comment ref="X6" authorId="1" shapeId="0" xr:uid="{4BB9E1A7-B022-46AE-9E98-BC8F14DC2BFC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -1661,7 +1688,7 @@
     from ChatGPT, need revision</t>
       </text>
     </comment>
-    <comment ref="P7" authorId="0" shapeId="0" xr:uid="{70D642DE-32B4-422D-B900-B8F154C15536}">
+    <comment ref="Q7" authorId="0" shapeId="0" xr:uid="{70D642DE-32B4-422D-B900-B8F154C15536}">
       <text>
         <r>
           <rPr>
@@ -1689,7 +1716,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q7" authorId="0" shapeId="0" xr:uid="{EEF463E6-46EB-4F38-A33E-3A2E4076E8BB}">
+    <comment ref="R7" authorId="0" shapeId="0" xr:uid="{EEF463E6-46EB-4F38-A33E-3A2E4076E8BB}">
       <text>
         <r>
           <rPr>
@@ -1816,7 +1843,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-[kW], maximum technology installation capacity</t>
+[kWh], maximum storage capacity</t>
         </r>
       </text>
     </comment>
@@ -2033,6 +2060,194 @@
           </rPr>
           <t xml:space="preserve">
 5 from MANGOret and 1.4 from the scaling factor between 2016 and 2022 from ASHP and GSHP</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Yiqiao Wang</author>
+  </authors>
+  <commentList>
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{81E1BE1C-7298-4630-BBC5-2F31D8814D57}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+in calliope, a dict with key as demand_electricity, value as timeseries df must be input during the initialization of the model.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{6851F39F-632B-4707-BA04-39C040A7267F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+might change based on the building's actual emission system.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{E01BE7B8-532E-4C30-80A0-602649AC7ABC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+might change based on the building's actual emission system.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{D17B07C3-6512-431D-9FED-6E0B731BCB93}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+might change based on the building's actual emission system.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Yiqiao Wang</author>
+  </authors>
+  <commentList>
+    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{93CD67AA-32CA-4C51-9086-92DA102085DB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+USD/m</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{1B0A58B6-B651-49C9-ADEB-8246D6FE8222}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+kgCO2eq/m</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{9C4FDEF2-EFB1-4EE8-92E6-0B85244A88D2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+[year]; if no monetary discount is wanted for future years, set the lifetime to 1.</t>
         </r>
       </text>
     </comment>
@@ -2041,7 +2256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="155">
   <si>
     <t>monetary</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2425,10 +2640,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>HEX_85_35</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>gas_micro_CHP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2518,6 +2729,131 @@
   </si>
   <si>
     <t>placeholder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>export</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-0.1460/-0.1022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>resource</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=supply_PV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=supply_SCET</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=supply_SCFP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand_electricity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand_space_cooling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand_hot_water</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>electrical_cable</t>
+  </si>
+  <si>
+    <t>#aeff60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#fac710</t>
+  </si>
+  <si>
+    <t>#12cdd4</t>
+  </si>
+  <si>
+    <t>#ff6728</t>
+  </si>
+  <si>
+    <t>demand</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cooling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=demand_electricity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=demand_space_heating</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=demand_space_cooling</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>df=demand_hot_water</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hot_water_pipe</t>
+  </si>
+  <si>
+    <t>cold_water_pipe</t>
+  </si>
+  <si>
+    <t>transmission</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>energy_con</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>energy_prod</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>purchase_per_distance</t>
+  </si>
+  <si>
+    <t>storage_cap_max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand_space_heating_35</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#fcd510</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#ffa210</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand_space_heating_60</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>demand_space_heating_85</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2603,7 +2939,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2624,6 +2960,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2971,7 +3310,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="V6" dT="2024-10-16T23:38:04.56" personId="{BAD9BABF-23D2-4A7A-A5F9-262A050E563D}" id="{4BB9E1A7-B022-46AE-9E98-BC8F14DC2BFC}">
+  <threadedComment ref="X6" dT="2024-10-16T23:38:04.56" personId="{BAD9BABF-23D2-4A7A-A5F9-262A050E563D}" id="{4BB9E1A7-B022-46AE-9E98-BC8F14DC2BFC}">
     <text>from ChatGPT, need revision</text>
   </threadedComment>
 </ThreadedComments>
@@ -2979,10 +3318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2603C43B-861B-457A-A24B-3EBFF53534AD}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -2994,40 +3333,43 @@
     <col min="5" max="5" width="12.9140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.9140625" customWidth="1"/>
     <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+    <row r="2" spans="1:9">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="7"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -3035,7 +3377,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>94</v>
@@ -3044,16 +3386,19 @@
         <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3061,7 +3406,7 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
@@ -3073,13 +3418,16 @@
         <v>0.05</v>
       </c>
       <c r="G4">
-        <v>2.4E-2</v>
+        <v>2.9100000000000001E-2</v>
       </c>
       <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3087,7 +3435,7 @@
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -3099,13 +3447,16 @@
         <v>0.05</v>
       </c>
       <c r="G5">
-        <v>1.6E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3113,7 +3464,7 @@
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
         <v>42</v>
@@ -3125,13 +3476,16 @@
         <v>0.05</v>
       </c>
       <c r="G6">
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
       <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -3139,7 +3493,7 @@
         <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" t="s">
         <v>43</v>
@@ -3154,10 +3508,13 @@
         <v>0.23</v>
       </c>
       <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3165,7 +3522,7 @@
         <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D8" t="s">
         <v>43</v>
@@ -3181,10 +3538,13 @@
         <v>0.17699999999999999</v>
       </c>
       <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -3192,7 +3552,7 @@
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D9" t="s">
         <v>43</v>
@@ -3207,10 +3567,13 @@
         <v>0.124</v>
       </c>
       <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -3218,7 +3581,7 @@
         <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
@@ -3233,10 +3596,13 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3244,7 +3610,7 @@
         <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" t="s">
         <v>19</v>
@@ -3259,10 +3625,13 @@
         <v>0.32400000000000001</v>
       </c>
       <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -3270,7 +3639,7 @@
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -3285,15 +3654,19 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="E1:G1"/>
+  <mergeCells count="5">
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="E1:H1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3303,10 +3676,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561E90E2-20B4-48EB-B5A5-7E82D5B88F8D}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -3316,63 +3689,72 @@
     <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.08203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.08203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="28.08203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -3380,7 +3762,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>94</v>
@@ -3389,37 +3771,46 @@
         <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="J3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="M3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="R3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3427,7 +3818,7 @@
         <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
@@ -3435,32 +3826,44 @@
       <c r="E4">
         <v>3000</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4">
         <v>0.05</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1250</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4" t="s">
         <v>89</v>
       </c>
-      <c r="K4">
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
         <v>5.56</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>42</v>
       </c>
-      <c r="N4">
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
         <v>10</v>
       </c>
-      <c r="O4">
+      <c r="R4">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3468,7 +3871,7 @@
         <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
         <v>42</v>
@@ -3476,38 +3879,47 @@
       <c r="E5">
         <v>1444</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5">
         <v>0.05</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>15555</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>1250</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
+        <v>126</v>
+      </c>
+      <c r="L5" t="s">
         <v>89</v>
       </c>
-      <c r="K5">
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
         <v>5.56</v>
       </c>
-      <c r="L5" t="s">
+      <c r="O5" t="s">
         <v>42</v>
       </c>
-      <c r="M5">
+      <c r="P5">
         <v>10</v>
       </c>
-      <c r="N5">
+      <c r="Q5">
         <v>100</v>
       </c>
-      <c r="O5">
+      <c r="R5">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3515,7 +3927,7 @@
         <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" t="s">
         <v>42</v>
@@ -3523,38 +3935,47 @@
       <c r="E6">
         <v>1000</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6">
         <v>0.05</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>6000</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>1250</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
+        <v>126</v>
+      </c>
+      <c r="L6" t="s">
         <v>89</v>
       </c>
-      <c r="K6">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
         <v>5.56</v>
       </c>
-      <c r="L6" t="s">
+      <c r="O6" t="s">
         <v>42</v>
       </c>
-      <c r="M6">
+      <c r="P6">
         <v>100</v>
       </c>
-      <c r="N6">
+      <c r="Q6">
         <v>200</v>
       </c>
-      <c r="O6">
+      <c r="R6">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3562,7 +3983,7 @@
         <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" t="s">
         <v>42</v>
@@ -3570,32 +3991,44 @@
       <c r="E7">
         <v>1300</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7">
         <v>0.05</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>1250</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>0</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
+        <v>126</v>
+      </c>
+      <c r="L7" t="s">
         <v>89</v>
       </c>
-      <c r="K7">
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
         <v>5.56</v>
       </c>
-      <c r="L7" t="s">
+      <c r="O7" t="s">
         <v>42</v>
       </c>
-      <c r="M7">
+      <c r="P7">
         <v>200</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
+        <v>2000</v>
+      </c>
+      <c r="R7">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -3603,7 +4036,7 @@
         <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8" t="s">
         <v>85</v>
@@ -3611,26 +4044,32 @@
       <c r="E8">
         <v>1576</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.05</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>290</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>0</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
+        <v>128</v>
+      </c>
+      <c r="L8" t="s">
         <v>89</v>
       </c>
-      <c r="K8">
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
         <v>2</v>
       </c>
-      <c r="O8">
+      <c r="R8">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -3638,7 +4077,7 @@
         <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D9" t="s">
         <v>58</v>
@@ -3646,49 +4085,61 @@
       <c r="E9">
         <v>2047</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.05</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>296</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
+        <v>127</v>
+      </c>
+      <c r="L9" t="s">
         <v>89</v>
       </c>
-      <c r="K9">
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
         <v>1.7</v>
       </c>
-      <c r="O9">
+      <c r="R9">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D10" t="s">
         <v>121</v>
       </c>
-      <c r="C10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" t="s">
-        <v>122</v>
-      </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.05</v>
       </c>
-      <c r="O10">
+      <c r="K10" t="s">
+        <v>125</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="R10">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="K1:R2"/>
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="J1:O2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3698,10 +4149,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A246388-C9BA-4771-92A8-398DB13C28C5}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -3724,48 +4175,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7" t="s">
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
@@ -3775,7 +4226,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>93</v>
@@ -3787,7 +4238,7 @@
         <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>21</v>
@@ -3799,7 +4250,7 @@
         <v>22</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>28</v>
@@ -3822,7 +4273,7 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -3869,7 +4320,7 @@
         <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -3916,7 +4367,7 @@
         <v>65</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -3963,7 +4414,7 @@
         <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -4010,7 +4461,7 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
         <v>42</v>
@@ -4057,7 +4508,7 @@
         <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
@@ -4084,7 +4535,7 @@
         <v>0</v>
       </c>
       <c r="L9">
-        <v>5.45</v>
+        <v>7.64</v>
       </c>
       <c r="M9">
         <v>5</v>
@@ -4104,7 +4555,7 @@
         <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
         <v>42</v>
@@ -4151,7 +4602,7 @@
         <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
         <v>42</v>
@@ -4178,7 +4629,7 @@
         <v>0</v>
       </c>
       <c r="L11">
-        <v>3.44</v>
+        <v>4.13</v>
       </c>
       <c r="M11">
         <v>5</v>
@@ -4198,7 +4649,7 @@
         <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" t="s">
         <v>42</v>
@@ -4245,7 +4696,7 @@
         <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D13" t="s">
         <v>42</v>
@@ -4272,7 +4723,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>2.6</v>
+        <v>2.96</v>
       </c>
       <c r="M13">
         <v>5</v>
@@ -4292,7 +4743,7 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D14" t="s">
         <v>43</v>
@@ -4339,7 +4790,7 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D15" t="s">
         <v>18</v>
@@ -4386,7 +4837,7 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D16" t="s">
         <v>19</v>
@@ -4433,7 +4884,7 @@
         <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D17" t="s">
         <v>43</v>
@@ -4480,7 +4931,7 @@
         <v>74</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D18" t="s">
         <v>18</v>
@@ -4527,7 +4978,7 @@
         <v>75</v>
       </c>
       <c r="C19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D19" t="s">
         <v>19</v>
@@ -4574,7 +5025,7 @@
         <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D20" t="s">
         <v>43</v>
@@ -4583,7 +5034,7 @@
         <v>58</v>
       </c>
       <c r="F20">
-        <v>155.3333333333334</v>
+        <v>155.333333333333</v>
       </c>
       <c r="G20">
         <v>0.05</v>
@@ -4621,7 +5072,7 @@
         <v>77</v>
       </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D21" t="s">
         <v>18</v>
@@ -4668,7 +5119,7 @@
         <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D22" t="s">
         <v>19</v>
@@ -4712,7 +5163,7 @@
         <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D23" t="s">
         <v>58</v>
@@ -4738,7 +5189,7 @@
         <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D24" t="s">
         <v>85</v>
@@ -4756,32 +5207,6 @@
         <v>1</v>
       </c>
       <c r="O24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15">
-      <c r="A25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C25" t="s">
-        <v>109</v>
-      </c>
-      <c r="D25" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" t="s">
-        <v>61</v>
-      </c>
-      <c r="G25">
-        <v>0.05</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>1</v>
-      </c>
-      <c r="O25">
         <v>1</v>
       </c>
     </row>
@@ -4801,10 +5226,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CCA624-D427-4AF6-862A-48646A94FFF1}">
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -4820,216 +5245,232 @@
     <col min="9" max="9" width="18.25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.58203125" customWidth="1"/>
-    <col min="16" max="16" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.08203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.58203125" customWidth="1"/>
+    <col min="17" max="17" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.25" customWidth="1"/>
+    <col min="22" max="22" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:24">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7" t="s">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7" t="s">
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+    </row>
+    <row r="2" spans="1:24">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7" t="s">
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="7"/>
-      <c r="V2" s="7"/>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="7" t="s">
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="I3" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="S4" s="9"/>
+      <c r="T4" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="U4" s="9"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="U5" s="9"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+    </row>
+    <row r="6" spans="1:24">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" t="s">
         <v>115</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="R4" s="8"/>
-      <c r="S4" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="R5" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="S5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="A6" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" t="s">
-        <v>116</v>
       </c>
       <c r="D6" t="s">
         <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J6">
         <v>1108.2</v>
@@ -5037,42 +5478,48 @@
       <c r="K6">
         <v>0.05</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="M6">
         <v>33195</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>1.1499999999999999</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>86.82</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>0</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <v>0.55000000000000004</v>
       </c>
-      <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="4">
+      <c r="S6" s="4"/>
+      <c r="T6" s="4">
         <v>0.64</v>
       </c>
-      <c r="T6">
+      <c r="U6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="V6">
         <v>10</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <v>500</v>
       </c>
-      <c r="V6">
+      <c r="X6">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D7" t="s">
         <v>42</v>
@@ -5092,42 +5539,43 @@
       <c r="K7">
         <v>0.05</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>55600</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>11.57</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>36.299999999999997</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>0</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>8</v>
       </c>
-      <c r="Q7" s="4">
-        <f>P7-1</f>
+      <c r="R7" s="4">
+        <f>Q7-1</f>
         <v>7</v>
       </c>
-      <c r="S7" s="4"/>
-      <c r="T7">
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7">
         <v>5</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <v>500</v>
       </c>
-      <c r="V7">
+      <c r="X7">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D8" t="s">
         <v>42</v>
@@ -5147,42 +5595,43 @@
       <c r="K8">
         <v>0.05</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>55600</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>11.57</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>36.299999999999997</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>0</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>4.4400000000000004</v>
       </c>
-      <c r="Q8" s="4">
-        <f>P8-1</f>
+      <c r="R8" s="4">
+        <f>Q8-1</f>
         <v>3.4400000000000004</v>
       </c>
-      <c r="S8" s="4"/>
-      <c r="T8">
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8">
         <v>5</v>
       </c>
-      <c r="U8">
+      <c r="W8">
         <v>500</v>
       </c>
-      <c r="V8">
+      <c r="X8">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
@@ -5202,64 +5651,66 @@
       <c r="K9">
         <v>0.05</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>55600</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>11.57</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>36.299999999999997</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>0</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <v>8</v>
       </c>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4">
-        <f>P9-1</f>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4">
+        <f>Q9-1</f>
         <v>7</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>5</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <v>500</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="28">
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="V3:V5"/>
+    <mergeCell ref="O3:O5"/>
+    <mergeCell ref="N3:N5"/>
+    <mergeCell ref="M3:M5"/>
+    <mergeCell ref="K3:K5"/>
+    <mergeCell ref="J3:J5"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="P3:P5"/>
+    <mergeCell ref="Q1:X2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="X3:X5"/>
+    <mergeCell ref="A1:I2"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
-    <mergeCell ref="P3:P5"/>
-    <mergeCell ref="U3:U5"/>
-    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="Q3:Q5"/>
+    <mergeCell ref="W3:W5"/>
+    <mergeCell ref="R4:S4"/>
     <mergeCell ref="I3:I5"/>
     <mergeCell ref="G3:G5"/>
     <mergeCell ref="F3:F5"/>
     <mergeCell ref="E3:E5"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="T3:T5"/>
-    <mergeCell ref="N3:N5"/>
-    <mergeCell ref="M3:M5"/>
     <mergeCell ref="L3:L5"/>
-    <mergeCell ref="K3:K5"/>
-    <mergeCell ref="J3:J5"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="O3:O5"/>
-    <mergeCell ref="P1:V2"/>
-    <mergeCell ref="J2:M2"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="V3:V5"/>
-    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="U3:U5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5271,8 +5722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED8072C-161B-4E9B-9246-F2F0563C6573}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="14"/>
@@ -5295,48 +5746,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7" t="s">
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
@@ -5346,7 +5797,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>16</v>
@@ -5358,28 +5809,28 @@
         <v>84</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>82</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>30</v>
+        <v>149</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>83</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>25</v>
@@ -5393,7 +5844,7 @@
         <v>38</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
@@ -5440,7 +5891,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" t="s">
         <v>61</v>
@@ -5484,7 +5935,7 @@
         <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
         <v>85</v>
@@ -5505,7 +5956,7 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="K6">
         <v>1000</v>
@@ -5528,7 +5979,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D7" t="s">
         <v>58</v>
@@ -5549,7 +6000,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0.96</v>
+        <v>0.94</v>
       </c>
       <c r="K7">
         <v>1000</v>
@@ -5576,4 +6027,372 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EC5F6A9-7225-4810-BBAF-71A9F1C444F7}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.08203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5DEC67-0815-4627-8893-747451CCD0D5}">
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.4140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.4140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10" customWidth="1"/>
+    <col min="11" max="11" width="7.58203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="I1:K2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E2:F2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
correct PV & SC efficiency
</commit_message>
<xml_diff>
--- a/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
+++ b/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangy\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D88AF50-DF68-49F7-9D92-E44A1CFE75DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11474CC-9D3B-4F47-A0AA-AC1DBDD74C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22046" yWindow="8649" windowWidth="22149" windowHeight="13200" activeTab="2" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
+    <workbookView xWindow="4650" yWindow="2480" windowWidth="31290" windowHeight="18200" activeTab="3" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
   </bookViews>
   <sheets>
     <sheet name="supply" sheetId="5" r:id="rId1"/>
@@ -545,6 +545,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{B542349D-BC24-4C65-A89F-1B47531CAF34}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1/0.771 from CEA database</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="O8" authorId="0" shapeId="0" xr:uid="{DD74A52F-1054-45EF-9073-B14456474A5B}">
       <text>
         <r>
@@ -637,7 +661,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-SCET has higher efficiency than SCFP.</t>
+1/0.71 from CEA database.</t>
         </r>
       </text>
     </comment>
@@ -3679,7 +3703,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -3848,7 +3872,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <v>5.56</v>
+        <v>5</v>
       </c>
       <c r="O4" t="s">
         <v>42</v>
@@ -3904,7 +3928,7 @@
         <v>1</v>
       </c>
       <c r="N5">
-        <v>5.56</v>
+        <v>5</v>
       </c>
       <c r="O5" t="s">
         <v>42</v>
@@ -3960,7 +3984,7 @@
         <v>1</v>
       </c>
       <c r="N6">
-        <v>5.56</v>
+        <v>5</v>
       </c>
       <c r="O6" t="s">
         <v>42</v>
@@ -4013,7 +4037,7 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <v>5.56</v>
+        <v>5</v>
       </c>
       <c r="O7" t="s">
         <v>42</v>
@@ -4063,7 +4087,7 @@
         <v>1</v>
       </c>
       <c r="N8">
-        <v>2</v>
+        <v>1.2969999999999999</v>
       </c>
       <c r="R8">
         <v>23</v>
@@ -4104,7 +4128,7 @@
         <v>1</v>
       </c>
       <c r="N9">
-        <v>1.7</v>
+        <v>1.41</v>
       </c>
       <c r="R9">
         <v>23</v>
@@ -4151,7 +4175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A246388-C9BA-4771-92A8-398DB13C28C5}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -5228,8 +5252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CCA624-D427-4AF6-862A-48646A94FFF1}">
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -5683,6 +5707,18 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="Q3:Q5"/>
+    <mergeCell ref="W3:W5"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="U3:U5"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="D3:D5"/>
@@ -5699,18 +5735,6 @@
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="X3:X5"/>
     <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="Q3:Q5"/>
-    <mergeCell ref="W3:W5"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="U3:U5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
preparing for sensitivity analysis (WIP)
</commit_message>
<xml_diff>
--- a/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
+++ b/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangy\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11474CC-9D3B-4F47-A0AA-AC1DBDD74C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC9B03D-00DE-482E-A785-55E40E3BBA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="2480" windowWidth="31290" windowHeight="18200" activeTab="3" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
   </bookViews>
   <sheets>
     <sheet name="supply" sheetId="5" r:id="rId1"/>
@@ -163,7 +163,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-bfe+wk palletten</t>
+bfe+wk palletten
+energie 360 suggests 0.08CHF/kWh on 11.4.2024</t>
         </r>
       </text>
     </comment>
@@ -3344,8 +3345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2603C43B-861B-457A-A24B-3EBFF53534AD}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -5252,8 +5253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CCA624-D427-4AF6-862A-48646A94FFF1}">
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -5707,18 +5708,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="Q3:Q5"/>
-    <mergeCell ref="W3:W5"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="U3:U5"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="D3:D5"/>
@@ -5735,6 +5724,18 @@
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="X3:X5"/>
     <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="Q3:Q5"/>
+    <mergeCell ref="W3:W5"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="U3:U5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
deleting some of integer decision variables to save computation time
</commit_message>
<xml_diff>
--- a/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
+++ b/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangy\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC9B03D-00DE-482E-A785-55E40E3BBA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7ACCAC-F8AC-4171-A651-BB10F992FE8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15943" activeTab="1" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
   </bookViews>
   <sheets>
     <sheet name="supply" sheetId="5" r:id="rId1"/>
@@ -276,32 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{6B6D44A3-5358-49C7-80BA-65B88BAD82BD}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-interception of installation cost curve
-[$/device]</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{381592D0-4B82-44EA-8DB3-F97383AB5D21}">
+    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{381592D0-4B82-44EA-8DB3-F97383AB5D21}">
       <text>
         <r>
           <rPr>
@@ -325,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{61312002-E024-4292-93F4-FD63A14A1DFD}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{61312002-E024-4292-93F4-FD63A14A1DFD}">
       <text>
         <r>
           <rPr>
@@ -350,7 +325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{A439E244-A83C-403E-BC74-150106BD9060}">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{A439E244-A83C-403E-BC74-150106BD9060}">
       <text>
         <r>
           <rPr>
@@ -374,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{F156C5E5-9988-454F-B199-E54895C12234}">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{F156C5E5-9988-454F-B199-E54895C12234}">
       <text>
         <r>
           <rPr>
@@ -398,7 +373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{AEFC007F-1ADD-4627-B6DF-D92185D067E3}">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{AEFC007F-1ADD-4627-B6DF-D92185D067E3}">
       <text>
         <r>
           <rPr>
@@ -422,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{164D751A-85F8-4A50-833D-EAAD0DAA59C2}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{164D751A-85F8-4A50-833D-EAAD0DAA59C2}">
       <text>
         <r>
           <rPr>
@@ -470,7 +445,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{637B0CCF-82B9-4C6D-A8BB-FCB6633100EF}">
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{637B0CCF-82B9-4C6D-A8BB-FCB6633100EF}">
       <text>
         <r>
           <rPr>
@@ -522,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{F8D9F75B-0547-4549-8288-A925727BEEAA}">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{F8D9F75B-0547-4549-8288-A925727BEEAA}">
       <text>
         <r>
           <rPr>
@@ -546,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{B542349D-BC24-4C65-A89F-1B47531CAF34}">
+    <comment ref="M8" authorId="0" shapeId="0" xr:uid="{B542349D-BC24-4C65-A89F-1B47531CAF34}">
       <text>
         <r>
           <rPr>
@@ -570,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{DD74A52F-1054-45EF-9073-B14456474A5B}">
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{DD74A52F-1054-45EF-9073-B14456474A5B}">
       <text>
         <r>
           <rPr>
@@ -594,7 +569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R8" authorId="0" shapeId="0" xr:uid="{2DCFA103-1274-4847-83A7-AC3F88F17291}">
+    <comment ref="Q8" authorId="0" shapeId="0" xr:uid="{2DCFA103-1274-4847-83A7-AC3F88F17291}">
       <text>
         <r>
           <rPr>
@@ -618,7 +593,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{27610EE9-A3A8-40CA-8A0D-BE26099C4505}">
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{27610EE9-A3A8-40CA-8A0D-BE26099C4505}">
       <text>
         <r>
           <rPr>
@@ -642,7 +617,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{BF918F83-D58B-46AA-AB83-02772C77D60C}">
+    <comment ref="M9" authorId="0" shapeId="0" xr:uid="{BF918F83-D58B-46AA-AB83-02772C77D60C}">
       <text>
         <r>
           <rPr>
@@ -666,7 +641,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R9" authorId="0" shapeId="0" xr:uid="{960AF645-C149-407D-B0B9-2EF4831D05BD}">
+    <comment ref="Q9" authorId="0" shapeId="0" xr:uid="{960AF645-C149-407D-B0B9-2EF4831D05BD}">
       <text>
         <r>
           <rPr>
@@ -1713,58 +1688,6 @@
     from ChatGPT, need revision</t>
       </text>
     </comment>
-    <comment ref="Q7" authorId="0" shapeId="0" xr:uid="{70D642DE-32B4-422D-B900-B8F154C15536}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-max(0.62*(60+273.15)/(60-35), 8)=8
-0.62: exergy efficiency
-60: high temperature
-35: low temperature
-8: normally the COP of current heat pump systems could not be higher than 8.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R7" authorId="0" shapeId="0" xr:uid="{EEF463E6-46EB-4F38-A33E-3A2E4076E8BB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-COP_L = CHP_H-1</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -2281,7 +2204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="152">
   <si>
     <t>monetary</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2730,18 +2653,6 @@
   </si>
   <si>
     <t>conversion_plus</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>booster_WSHP_35_60</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>booster_WSHP_35_85</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>booster_WSHP_60_85</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3345,21 +3256,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2603C43B-861B-457A-A24B-3EBFF53534AD}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.9140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.9140625" customWidth="1"/>
-    <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.92578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.92578125" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -3701,35 +3612,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561E90E2-20B4-48EB-B5A5-7E82D5B88F8D}">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="12.9140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="28.08203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.08203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.92578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
+    <col min="13" max="13" width="28.0703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.2109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.0703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:17">
       <c r="A1" s="8" t="s">
         <v>14</v>
       </c>
@@ -3743,19 +3653,18 @@
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>27</v>
       </c>
+      <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-    </row>
-    <row r="2" spans="1:18">
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -3765,10 +3674,10 @@
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -3777,9 +3686,8 @@
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-    </row>
-    <row r="3" spans="1:18">
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -3796,46 +3704,43 @@
         <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>111</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>124</v>
+        <v>87</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>87</v>
+        <v>28</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -3852,43 +3757,43 @@
         <v>3000</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G4">
         <v>0.05</v>
       </c>
+      <c r="H4">
+        <v>1250</v>
+      </c>
       <c r="I4">
-        <v>1250</v>
-      </c>
-      <c r="J4">
         <v>0</v>
       </c>
+      <c r="J4" t="s">
+        <v>123</v>
+      </c>
       <c r="K4" t="s">
-        <v>126</v>
-      </c>
-      <c r="L4" t="s">
         <v>89</v>
       </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
       <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
         <v>5</v>
       </c>
-      <c r="O4" t="s">
+      <c r="N4" t="s">
         <v>42</v>
       </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
       <c r="P4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q4">
-        <v>10</v>
-      </c>
-      <c r="R4">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -3902,49 +3807,46 @@
         <v>42</v>
       </c>
       <c r="E5">
-        <v>1444</v>
+        <v>2200</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G5">
         <v>0.05</v>
       </c>
       <c r="H5">
-        <v>15555</v>
+        <v>1250</v>
       </c>
       <c r="I5">
-        <v>1250</v>
-      </c>
-      <c r="J5">
         <v>0</v>
       </c>
+      <c r="J5" t="s">
+        <v>123</v>
+      </c>
       <c r="K5" t="s">
-        <v>126</v>
-      </c>
-      <c r="L5" t="s">
         <v>89</v>
       </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
       <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
         <v>5</v>
       </c>
-      <c r="O5" t="s">
+      <c r="N5" t="s">
         <v>42</v>
       </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
       <c r="P5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="Q5">
-        <v>100</v>
-      </c>
-      <c r="R5">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3958,49 +3860,46 @@
         <v>42</v>
       </c>
       <c r="E6">
-        <v>1000</v>
+        <v>1600</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G6">
         <v>0.05</v>
       </c>
       <c r="H6">
-        <v>6000</v>
+        <v>1250</v>
       </c>
       <c r="I6">
-        <v>1250</v>
-      </c>
-      <c r="J6">
         <v>0</v>
       </c>
+      <c r="J6" t="s">
+        <v>123</v>
+      </c>
       <c r="K6" t="s">
-        <v>126</v>
-      </c>
-      <c r="L6" t="s">
         <v>89</v>
       </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
       <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
         <v>5</v>
       </c>
-      <c r="O6" t="s">
+      <c r="N6" t="s">
         <v>42</v>
       </c>
+      <c r="O6">
+        <v>100</v>
+      </c>
       <c r="P6">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="Q6">
-        <v>200</v>
-      </c>
-      <c r="R6">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -4017,43 +3916,43 @@
         <v>1300</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G7">
         <v>0.05</v>
       </c>
+      <c r="H7">
+        <v>1250</v>
+      </c>
       <c r="I7">
-        <v>1250</v>
-      </c>
-      <c r="J7">
         <v>0</v>
       </c>
+      <c r="J7" t="s">
+        <v>123</v>
+      </c>
       <c r="K7" t="s">
-        <v>126</v>
-      </c>
-      <c r="L7" t="s">
         <v>89</v>
       </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
       <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
         <v>5</v>
       </c>
-      <c r="O7" t="s">
+      <c r="N7" t="s">
         <v>42</v>
       </c>
+      <c r="O7">
+        <v>200</v>
+      </c>
       <c r="P7">
-        <v>200</v>
+        <v>2000</v>
       </c>
       <c r="Q7">
-        <v>2000</v>
-      </c>
-      <c r="R7">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -4072,29 +3971,29 @@
       <c r="G8">
         <v>0.05</v>
       </c>
+      <c r="H8">
+        <v>290</v>
+      </c>
       <c r="I8">
-        <v>290</v>
-      </c>
-      <c r="J8">
         <v>0</v>
       </c>
+      <c r="J8" t="s">
+        <v>125</v>
+      </c>
       <c r="K8" t="s">
-        <v>128</v>
-      </c>
-      <c r="L8" t="s">
         <v>89</v>
       </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
       <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8">
         <v>1.2969999999999999</v>
       </c>
-      <c r="R8">
+      <c r="Q8">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>91</v>
       </c>
@@ -4113,58 +4012,58 @@
       <c r="G9">
         <v>0.05</v>
       </c>
+      <c r="H9">
+        <v>296</v>
+      </c>
       <c r="I9">
-        <v>296</v>
-      </c>
-      <c r="J9">
         <v>0</v>
       </c>
+      <c r="J9" t="s">
+        <v>124</v>
+      </c>
       <c r="K9" t="s">
-        <v>127</v>
-      </c>
-      <c r="L9" t="s">
         <v>89</v>
       </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
       <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
         <v>1.41</v>
       </c>
-      <c r="R9">
+      <c r="Q9">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
         <v>106</v>
       </c>
       <c r="D10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G10">
         <v>0.05</v>
       </c>
-      <c r="K10" t="s">
-        <v>125</v>
-      </c>
-      <c r="M10">
+      <c r="J10" t="s">
+        <v>122</v>
+      </c>
+      <c r="L10">
         <v>1</v>
       </c>
-      <c r="R10">
+      <c r="Q10">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="K1:R2"/>
+    <mergeCell ref="J1:Q2"/>
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4180,23 +4079,23 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" customWidth="1"/>
-    <col min="12" max="12" width="10.08203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.0703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.0703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -5251,37 +5150,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CCA624-D427-4AF6-862A-48646A94FFF1}">
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.2109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.58203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.58203125" customWidth="1"/>
-    <col min="17" max="17" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.25" customWidth="1"/>
-    <col min="22" max="22" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10.2109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.2109375" customWidth="1"/>
+    <col min="22" max="22" width="15.0703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -5381,7 +5280,7 @@
         <v>111</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>21</v>
@@ -5399,7 +5298,7 @@
         <v>28</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
@@ -5504,7 +5403,7 @@
         <v>0.05</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="M6">
         <v>33195</v>
@@ -5539,175 +5438,20 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
-      <c r="A7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" t="s">
-        <v>85</v>
-      </c>
-      <c r="J7">
-        <v>1113.5999999999999</v>
-      </c>
-      <c r="K7">
-        <v>0.05</v>
-      </c>
-      <c r="M7">
-        <v>55600</v>
-      </c>
-      <c r="N7">
-        <v>11.57</v>
-      </c>
-      <c r="O7">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>8</v>
-      </c>
-      <c r="R7" s="4">
-        <f>Q7-1</f>
-        <v>7</v>
-      </c>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7">
-        <v>5</v>
-      </c>
-      <c r="W7">
-        <v>500</v>
-      </c>
-      <c r="X7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24">
-      <c r="A8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" t="s">
-        <v>61</v>
-      </c>
-      <c r="F8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" t="s">
-        <v>58</v>
-      </c>
-      <c r="J8">
-        <v>1113.5999999999999</v>
-      </c>
-      <c r="K8">
-        <v>0.05</v>
-      </c>
-      <c r="M8">
-        <v>55600</v>
-      </c>
-      <c r="N8">
-        <v>11.57</v>
-      </c>
-      <c r="O8">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>4.4400000000000004</v>
-      </c>
-      <c r="R8" s="4">
-        <f>Q8-1</f>
-        <v>3.4400000000000004</v>
-      </c>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8">
-        <v>5</v>
-      </c>
-      <c r="W8">
-        <v>500</v>
-      </c>
-      <c r="X8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24">
-      <c r="A9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C9" t="s">
-        <v>115</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9">
-        <v>1113.5999999999999</v>
-      </c>
-      <c r="K9">
-        <v>0.05</v>
-      </c>
-      <c r="M9">
-        <v>55600</v>
-      </c>
-      <c r="N9">
-        <v>11.57</v>
-      </c>
-      <c r="O9">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>8</v>
-      </c>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4">
-        <f>Q9-1</f>
-        <v>7</v>
-      </c>
-      <c r="V9">
-        <v>5</v>
-      </c>
-      <c r="W9">
-        <v>500</v>
-      </c>
-      <c r="X9">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="Q3:Q5"/>
+    <mergeCell ref="W3:W5"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="U3:U5"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="D3:D5"/>
@@ -5724,18 +5468,6 @@
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="X3:X5"/>
     <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="Q3:Q5"/>
-    <mergeCell ref="W3:W5"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="U3:U5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5751,23 +5483,23 @@
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.4140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.4140625" customWidth="1"/>
-    <col min="10" max="10" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.0703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.08203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.0703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.2109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -5846,7 +5578,7 @@
         <v>28</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>83</v>
@@ -6062,13 +5794,13 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.35546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.2109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.0703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6103,109 +5835,109 @@
         <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" t="s">
         <v>134</v>
-      </c>
-      <c r="C5" t="s">
-        <v>137</v>
       </c>
       <c r="D5" t="s">
         <v>61</v>
       </c>
       <c r="E5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D6" t="s">
         <v>85</v>
       </c>
       <c r="E6" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D7" t="s">
         <v>58</v>
       </c>
       <c r="E7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" t="s">
         <v>135</v>
       </c>
-      <c r="C8" t="s">
-        <v>137</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>138</v>
-      </c>
-      <c r="E8" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D9" t="s">
         <v>85</v>
       </c>
       <c r="E9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -6227,18 +5959,18 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.35546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.0703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.4140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.4140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.640625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -6291,22 +6023,22 @@
         <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>111</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>111</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>25</v>
@@ -6314,10 +6046,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
@@ -6346,10 +6078,10 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
         <v>58</v>
@@ -6378,10 +6110,10 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>

</xml_diff>

<commit_message>
update technology definition to correctly consider PV technologies
</commit_message>
<xml_diff>
--- a/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
+++ b/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangy\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7ACCAC-F8AC-4171-A651-BB10F992FE8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E016CD50-71A5-4FFB-B25A-1ED5EBF214F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15943" activeTab="1" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
   </bookViews>
   <sheets>
     <sheet name="supply" sheetId="5" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="conversion_plus" sheetId="10" r:id="rId4"/>
     <sheet name="storage" sheetId="8" r:id="rId5"/>
     <sheet name="demand" sheetId="11" r:id="rId6"/>
-    <sheet name="transmission" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -95,31 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{BB037499-8E99-4383-B813-7D1DE03BA999}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-ewz</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G7" authorId="0" shapeId="0" xr:uid="{5F07713E-B53A-4F68-B948-0DE6093B4E37}">
+    <comment ref="G5" authorId="0" shapeId="0" xr:uid="{5F07713E-B53A-4F68-B948-0DE6093B4E37}">
       <text>
         <r>
           <rPr>
@@ -143,7 +118,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{29079865-22BD-4294-8AAF-CA614A3F9A35}">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{29079865-22BD-4294-8AAF-CA614A3F9A35}">
       <text>
         <r>
           <rPr>
@@ -168,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{33A05C13-4314-4914-82EE-E11B048CC5C7}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{33A05C13-4314-4914-82EE-E11B048CC5C7}">
       <text>
         <r>
           <rPr>
@@ -192,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{B664C2FD-AA61-4A19-91B5-C6D3502ACED2}">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{B664C2FD-AA61-4A19-91B5-C6D3502ACED2}">
       <text>
         <r>
           <rPr>
@@ -217,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{F979F4B1-5E70-4C02-B7AD-A61C2F5CB7BC}">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{F979F4B1-5E70-4C02-B7AD-A61C2F5CB7BC}">
       <text>
         <r>
           <rPr>
@@ -276,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{381592D0-4B82-44EA-8DB3-F97383AB5D21}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{381592D0-4B82-44EA-8DB3-F97383AB5D21}">
       <text>
         <r>
           <rPr>
@@ -300,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{61312002-E024-4292-93F4-FD63A14A1DFD}">
+    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{61312002-E024-4292-93F4-FD63A14A1DFD}">
       <text>
         <r>
           <rPr>
@@ -325,7 +300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{A439E244-A83C-403E-BC74-150106BD9060}">
+    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{A439E244-A83C-403E-BC74-150106BD9060}">
       <text>
         <r>
           <rPr>
@@ -349,7 +324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O3" authorId="0" shapeId="0" xr:uid="{F156C5E5-9988-454F-B199-E54895C12234}">
+    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{F156C5E5-9988-454F-B199-E54895C12234}">
       <text>
         <r>
           <rPr>
@@ -373,7 +348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{AEFC007F-1ADD-4627-B6DF-D92185D067E3}">
+    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{AEFC007F-1ADD-4627-B6DF-D92185D067E3}">
       <text>
         <r>
           <rPr>
@@ -397,7 +372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0" xr:uid="{164D751A-85F8-4A50-833D-EAAD0DAA59C2}">
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{164D751A-85F8-4A50-833D-EAAD0DAA59C2}">
       <text>
         <r>
           <rPr>
@@ -445,7 +420,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{637B0CCF-82B9-4C6D-A8BB-FCB6633100EF}">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{70DFC5FF-1C68-4CF5-9BFD-C4F9FAC59057}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+just adding binary variable to technology. This somehow helps with model feasibility.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{637B0CCF-82B9-4C6D-A8BB-FCB6633100EF}">
       <text>
         <r>
           <rPr>
@@ -469,7 +468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{E12426D1-3981-473D-8372-399B69C9CB5F}">
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{E12426D1-3981-473D-8372-399B69C9CB5F}">
       <text>
         <r>
           <rPr>
@@ -497,7 +496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{F8D9F75B-0547-4549-8288-A925727BEEAA}">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{F8D9F75B-0547-4549-8288-A925727BEEAA}">
       <text>
         <r>
           <rPr>
@@ -521,7 +520,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M8" authorId="0" shapeId="0" xr:uid="{B542349D-BC24-4C65-A89F-1B47531CAF34}">
+    <comment ref="N7" authorId="0" shapeId="0" xr:uid="{B542349D-BC24-4C65-A89F-1B47531CAF34}">
       <text>
         <r>
           <rPr>
@@ -545,7 +544,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{DD74A52F-1054-45EF-9073-B14456474A5B}">
+    <comment ref="O7" authorId="0" shapeId="0" xr:uid="{DD74A52F-1054-45EF-9073-B14456474A5B}">
       <text>
         <r>
           <rPr>
@@ -569,7 +568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q8" authorId="0" shapeId="0" xr:uid="{2DCFA103-1274-4847-83A7-AC3F88F17291}">
+    <comment ref="R7" authorId="0" shapeId="0" xr:uid="{2DCFA103-1274-4847-83A7-AC3F88F17291}">
       <text>
         <r>
           <rPr>
@@ -593,7 +592,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{27610EE9-A3A8-40CA-8A0D-BE26099C4505}">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{27610EE9-A3A8-40CA-8A0D-BE26099C4505}">
       <text>
         <r>
           <rPr>
@@ -617,7 +616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M9" authorId="0" shapeId="0" xr:uid="{BF918F83-D58B-46AA-AB83-02772C77D60C}">
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{BF918F83-D58B-46AA-AB83-02772C77D60C}">
       <text>
         <r>
           <rPr>
@@ -641,7 +640,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q9" authorId="0" shapeId="0" xr:uid="{960AF645-C149-407D-B0B9-2EF4831D05BD}">
+    <comment ref="R8" authorId="0" shapeId="0" xr:uid="{960AF645-C149-407D-B0B9-2EF4831D05BD}">
       <text>
         <r>
           <rPr>
@@ -662,30 +661,6 @@
           </rPr>
           <t xml:space="preserve">
 danish solar heating, average single/apart</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{58ABB07C-8821-40E3-8620-1B9FF3CEFAEF}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-just a placeholder for now.</t>
         </r>
       </text>
     </comment>
@@ -2121,111 +2096,13 @@
 </comments>
 </file>
 
-<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Yiqiao Wang</author>
-  </authors>
-  <commentList>
-    <comment ref="E3" authorId="0" shapeId="0" xr:uid="{93CD67AA-32CA-4C51-9086-92DA102085DB}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-USD/m</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="0" shapeId="0" xr:uid="{1B0A58B6-B651-49C9-ADEB-8246D6FE8222}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-kgCO2eq/m</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{9C4FDEF2-EFB1-4EE8-92E6-0B85244A88D2}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-[year]; if no monetary discount is wanted for future years, set the lifetime to 1.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="137">
   <si>
     <t>monetary</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>electricity_pronatur</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>electricity_natur</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.3189/0.2048</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.3016/0.1876</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0.2994/0.1854</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2258,10 +2135,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PV_extra_large</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>essentials</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2342,10 +2215,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#19c869</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>#094926</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2561,9 +2430,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#c69874</t>
-  </si>
-  <si>
     <t>carrier_in</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2660,14 +2526,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PVT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>placeholder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>export</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2680,10 +2538,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>df=</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>df=supply_PV</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2708,9 +2562,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>electrical_cable</t>
-  </si>
-  <si>
     <t>#aeff60</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2748,27 +2599,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>hot_water_pipe</t>
-  </si>
-  <si>
-    <t>cold_water_pipe</t>
-  </si>
-  <si>
-    <t>transmission</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>energy_con</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>energy_prod</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>purchase_per_distance</t>
-  </si>
-  <si>
     <t>storage_cap_max</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2790,6 +2620,14 @@
   </si>
   <si>
     <t>demand_space_heating_85</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>force_resource</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>purchase</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3254,40 +3092,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2603C43B-861B-457A-A24B-3EBFF53534AD}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.35546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.92578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.92578125" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.9140625" customWidth="1"/>
+    <col min="7" max="7" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3300,61 +3138,61 @@
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
         <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
       </c>
       <c r="F4">
         <v>0.05</v>
       </c>
       <c r="G4">
-        <v>2.9100000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -3365,25 +3203,25 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
+        <v>37</v>
+      </c>
+      <c r="E5">
+        <v>0.13250000000000001</v>
       </c>
       <c r="F5">
         <v>0.05</v>
       </c>
       <c r="G5">
-        <v>2.1000000000000001E-2</v>
+        <v>0.23</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -3394,25 +3232,26 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
+        <v>37</v>
+      </c>
+      <c r="E6">
+        <v>0.14299999999999999</v>
       </c>
       <c r="F6">
         <v>0.05</v>
       </c>
       <c r="G6">
-        <v>0.02</v>
+        <f>AVERAGE(G5,G7)</f>
+        <v>0.17699999999999999</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3423,25 +3262,25 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" t="s">
-        <v>43</v>
-      </c>
       <c r="E7">
-        <v>0.13250000000000001</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="F7">
         <v>0.05</v>
       </c>
       <c r="G7">
-        <v>0.23</v>
+        <v>0.124</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -3452,26 +3291,25 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E8">
-        <v>0.14299999999999999</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="F8">
         <v>0.05</v>
       </c>
       <c r="G8">
-        <f>AVERAGE(G7,G9)</f>
-        <v>0.17699999999999999</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -3482,25 +3320,25 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="E9">
-        <v>0.17799999999999999</v>
+        <v>0.1</v>
       </c>
       <c r="F9">
         <v>0.05</v>
       </c>
       <c r="G9">
-        <v>0.124</v>
+        <v>0.32400000000000001</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -3511,88 +3349,30 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E10">
-        <v>0.10199999999999999</v>
+        <v>0.122</v>
       </c>
       <c r="F10">
         <v>0.05</v>
       </c>
       <c r="G10">
-        <v>2.8000000000000001E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11">
-        <v>0.1</v>
-      </c>
-      <c r="F11">
-        <v>0.05</v>
-      </c>
-      <c r="G11">
-        <v>0.32400000000000001</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12">
-        <v>0.122</v>
-      </c>
-      <c r="F12">
-        <v>0.05</v>
-      </c>
-      <c r="G12">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
         <v>1</v>
       </c>
     </row>
@@ -3612,59 +3392,61 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{561E90E2-20B4-48EB-B5A5-7E82D5B88F8D}">
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="12.92578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.35546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5" customWidth="1"/>
-    <col min="13" max="13" width="28.0703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.2109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.0703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.1640625" customWidth="1"/>
+    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.08203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.08203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="8"/>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -3674,10 +3456,10 @@
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -3686,384 +3468,333 @@
       <c r="O2" s="8"/>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" s="8"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>111</v>
+        <v>17</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>28</v>
+        <v>135</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>3000</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="G4">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4">
         <v>0.05</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1250</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0</v>
       </c>
-      <c r="J4" t="s">
-        <v>123</v>
-      </c>
       <c r="K4" t="s">
-        <v>89</v>
-      </c>
-      <c r="L4">
+        <v>113</v>
+      </c>
+      <c r="L4" t="b">
         <v>1</v>
       </c>
-      <c r="M4">
+      <c r="M4" t="s">
+        <v>83</v>
+      </c>
+      <c r="N4">
         <v>5</v>
       </c>
-      <c r="N4" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4">
+      <c r="O4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>10</v>
+      </c>
+      <c r="R4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5">
+        <v>1444</v>
+      </c>
+      <c r="F5">
+        <v>15555.6</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H5">
+        <v>0.05</v>
+      </c>
+      <c r="I5">
+        <v>1250</v>
+      </c>
+      <c r="J5">
         <v>0</v>
       </c>
-      <c r="P4">
+      <c r="K5" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>83</v>
+      </c>
+      <c r="N5">
+        <v>5</v>
+      </c>
+      <c r="O5" t="s">
+        <v>36</v>
+      </c>
+      <c r="P5">
         <v>10</v>
       </c>
-      <c r="Q4">
+      <c r="Q5">
+        <v>100</v>
+      </c>
+      <c r="R5">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5">
-        <v>2200</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="G5">
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6">
+        <v>1284</v>
+      </c>
+      <c r="F6">
+        <v>31579</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6">
         <v>0.05</v>
       </c>
-      <c r="H5">
+      <c r="I6">
         <v>1250</v>
       </c>
-      <c r="I5">
+      <c r="J6">
         <v>0</v>
       </c>
-      <c r="J5" t="s">
-        <v>123</v>
-      </c>
-      <c r="K5" t="s">
-        <v>89</v>
-      </c>
-      <c r="L5">
+      <c r="K6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L6" t="b">
         <v>1</v>
       </c>
-      <c r="M5">
+      <c r="M6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N6">
         <v>5</v>
       </c>
-      <c r="N5" t="s">
-        <v>42</v>
-      </c>
-      <c r="O5">
-        <v>10</v>
-      </c>
-      <c r="P5">
+      <c r="O6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6">
         <v>100</v>
       </c>
-      <c r="Q5">
+      <c r="Q6">
+        <v>2000</v>
+      </c>
+      <c r="R6">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6">
-        <v>1600</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="G6">
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7">
+        <v>1576</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>0.05</v>
       </c>
-      <c r="H6">
-        <v>1250</v>
-      </c>
-      <c r="I6">
+      <c r="I7">
+        <v>290</v>
+      </c>
+      <c r="J7">
         <v>0</v>
       </c>
-      <c r="J6" t="s">
-        <v>123</v>
-      </c>
-      <c r="K6" t="s">
-        <v>89</v>
-      </c>
-      <c r="L6">
+      <c r="K7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L7" t="b">
         <v>1</v>
       </c>
-      <c r="M6">
-        <v>5</v>
-      </c>
-      <c r="N6" t="s">
-        <v>42</v>
-      </c>
-      <c r="O6">
+      <c r="M7" t="s">
+        <v>83</v>
+      </c>
+      <c r="N7">
+        <v>1.2969999999999999</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
         <v>100</v>
       </c>
-      <c r="P6">
-        <v>200</v>
-      </c>
-      <c r="Q6">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7">
-        <v>1300</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="G7">
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <v>2047</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="H8">
         <v>0.05</v>
       </c>
-      <c r="H7">
-        <v>1250</v>
-      </c>
-      <c r="I7">
+      <c r="I8">
+        <v>296</v>
+      </c>
+      <c r="J8">
         <v>0</v>
       </c>
-      <c r="J7" t="s">
-        <v>123</v>
-      </c>
-      <c r="K7" t="s">
-        <v>89</v>
-      </c>
-      <c r="L7">
+      <c r="K8" t="s">
+        <v>114</v>
+      </c>
+      <c r="L8" t="b">
         <v>1</v>
       </c>
-      <c r="M7">
-        <v>5</v>
-      </c>
-      <c r="N7" t="s">
-        <v>42</v>
-      </c>
-      <c r="O7">
-        <v>200</v>
-      </c>
-      <c r="P7">
-        <v>2000</v>
-      </c>
-      <c r="Q7">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8">
-        <v>1576</v>
-      </c>
-      <c r="G8">
-        <v>0.05</v>
-      </c>
-      <c r="H8">
-        <v>290</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8" t="s">
-        <v>125</v>
-      </c>
-      <c r="K8" t="s">
-        <v>89</v>
-      </c>
-      <c r="L8">
+      <c r="M8" t="s">
+        <v>83</v>
+      </c>
+      <c r="N8">
+        <v>1.41</v>
+      </c>
+      <c r="P8">
         <v>1</v>
       </c>
-      <c r="M8">
-        <v>1.2969999999999999</v>
-      </c>
-      <c r="Q8">
+      <c r="R8">
         <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9">
-        <v>2047</v>
-      </c>
-      <c r="G9">
-        <v>0.05</v>
-      </c>
-      <c r="H9">
-        <v>296</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9" t="s">
-        <v>124</v>
-      </c>
-      <c r="K9" t="s">
-        <v>89</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9">
-        <v>1.41</v>
-      </c>
-      <c r="Q9">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" t="s">
-        <v>118</v>
-      </c>
-      <c r="G10">
-        <v>0.05</v>
-      </c>
-      <c r="J10" t="s">
-        <v>122</v>
-      </c>
-      <c r="L10">
-        <v>1</v>
-      </c>
-      <c r="Q10">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="J1:Q2"/>
+    <mergeCell ref="K1:R2"/>
     <mergeCell ref="A1:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E1:I1"/>
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4076,38 +3807,38 @@
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.35546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.2109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.2109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" customWidth="1"/>
-    <col min="12" max="12" width="10.0703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.0703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10.08203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.08203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -4115,7 +3846,7 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
@@ -4134,7 +3865,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -4144,66 +3875,66 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="L3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="M3" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F4">
         <v>371.80000000000013</v>
@@ -4238,19 +3969,19 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F5">
         <v>180.88</v>
@@ -4285,28 +4016,28 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F6">
-        <v>117.36666666666666</v>
+        <v>117.4</v>
       </c>
       <c r="G6">
         <v>0.05</v>
       </c>
       <c r="H6">
-        <v>29571.666666666672</v>
+        <v>29571.7</v>
       </c>
       <c r="I6">
         <v>150</v>
@@ -4332,19 +4063,19 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F7">
         <v>72.010000000000005</v>
@@ -4379,19 +4110,19 @@
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F8">
         <v>1814.5</v>
@@ -4426,19 +4157,19 @@
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F9">
         <v>2544.9</v>
@@ -4473,19 +4204,19 @@
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F10">
         <v>1814.5</v>
@@ -4520,19 +4251,19 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F11">
         <v>2544.9</v>
@@ -4567,19 +4298,19 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F12">
         <v>1814.5</v>
@@ -4614,19 +4345,19 @@
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F13">
         <v>2544.9</v>
@@ -4661,19 +4392,19 @@
     </row>
     <row r="14" spans="1:15">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F14">
         <v>300</v>
@@ -4708,19 +4439,19 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F15">
         <v>880</v>
@@ -4755,28 +4486,28 @@
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F16">
-        <v>486.66666666666669</v>
+        <v>486.7</v>
       </c>
       <c r="G16">
         <v>0.05</v>
       </c>
       <c r="H16">
-        <v>20466.666666666664</v>
+        <v>20466.7</v>
       </c>
       <c r="I16">
         <v>3.5</v>
@@ -4802,28 +4533,28 @@
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F17">
-        <v>176.66666666666666</v>
+        <v>176.7</v>
       </c>
       <c r="G17">
         <v>0.05</v>
       </c>
       <c r="H17">
-        <v>19666.666666666668</v>
+        <v>19666.7</v>
       </c>
       <c r="I17">
         <v>6.3</v>
@@ -4849,19 +4580,19 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
         <v>52</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C18" t="s">
-        <v>108</v>
-      </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" t="s">
-        <v>58</v>
       </c>
       <c r="F18">
         <v>414.99999999999989</v>
@@ -4896,28 +4627,28 @@
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F19">
-        <v>189.44444444444443</v>
+        <v>189.4</v>
       </c>
       <c r="G19">
         <v>0.05</v>
       </c>
       <c r="H19">
-        <v>26411.111111111113</v>
+        <v>26411.1</v>
       </c>
       <c r="I19">
         <v>3.5</v>
@@ -4943,28 +4674,28 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F20">
-        <v>155.333333333333</v>
+        <v>155.30000000000001</v>
       </c>
       <c r="G20">
         <v>0.05</v>
       </c>
       <c r="H20">
-        <v>23933.333333333307</v>
+        <v>23933.3</v>
       </c>
       <c r="I20">
         <v>6.3</v>
@@ -4990,19 +4721,19 @@
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C21" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F21">
         <v>278.00000000000006</v>
@@ -5037,28 +4768,28 @@
     </row>
     <row r="22" spans="1:15">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="F22">
-        <v>211.66666666666666</v>
+        <v>211.7</v>
       </c>
       <c r="G22">
         <v>0.05</v>
       </c>
       <c r="H22">
-        <v>21966.666666666672</v>
+        <v>21966.7</v>
       </c>
       <c r="I22">
         <v>3.5</v>
@@ -5084,16 +4815,16 @@
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G23">
         <v>0.05</v>
@@ -5110,16 +4841,16 @@
     </row>
     <row r="24" spans="1:15">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G24">
         <v>0.05</v>
@@ -5152,40 +4883,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5CCA624-D427-4AF6-862A-48646A94FFF1}">
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.35546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.2109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.2109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" customWidth="1"/>
-    <col min="17" max="17" width="10.2109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.2109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.2109375" customWidth="1"/>
-    <col min="22" max="22" width="15.0703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.58203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.58203125" customWidth="1"/>
+    <col min="17" max="17" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.25" customWidth="1"/>
+    <col min="22" max="22" width="15.08203125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
       <c r="A1" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -5196,7 +4927,7 @@
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -5205,7 +4936,7 @@
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
       <c r="Q1" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
@@ -5233,7 +4964,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -5247,72 +4978,72 @@
     </row>
     <row r="3" spans="1:24">
       <c r="A3" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>100</v>
-      </c>
       <c r="F3" s="8" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="G3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="N3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="R3" s="9" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
       <c r="U3" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="V3" s="8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="W3" s="8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="X3" s="8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -5334,11 +5065,11 @@
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="9" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="S4" s="9"/>
       <c r="T4" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="U4" s="9"/>
       <c r="V4" s="8"/>
@@ -5364,13 +5095,13 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="U5" s="9"/>
       <c r="V5" s="8"/>
@@ -5379,22 +5110,22 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="I6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="J6">
         <v>1108.2</v>
@@ -5403,7 +5134,7 @@
         <v>0.05</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="M6">
         <v>33195</v>
@@ -5426,7 +5157,7 @@
         <v>0.64</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="V6">
         <v>10</v>
@@ -5479,45 +5210,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ED8072C-161B-4E9B-9246-F2F0563C6573}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.4140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.0703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.4140625" customWidth="1"/>
+    <col min="10" max="10" width="10.08203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.0703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.2109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -5536,7 +5267,7 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
@@ -5548,63 +5279,63 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>110</v>
-      </c>
       <c r="O3" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>367</v>
@@ -5642,16 +5373,16 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <v>13</v>
@@ -5686,16 +5417,16 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E6">
         <v>13</v>
@@ -5730,16 +5461,16 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E7">
         <v>13</v>
@@ -5791,27 +5522,27 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="23.35546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.2109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.0703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -5823,121 +5554,121 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E6" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E7" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8" t="s">
         <v>127</v>
-      </c>
-      <c r="B8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D8" t="s">
-        <v>135</v>
-      </c>
-      <c r="E8" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" t="s">
         <v>128</v>
-      </c>
-      <c r="B9" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -5949,207 +5680,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5DEC67-0815-4627-8893-747451CCD0D5}">
-  <dimension ref="A1:K6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15"/>
-  <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.35546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.0703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10" customWidth="1"/>
-    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C6" t="s">
-        <v>142</v>
-      </c>
-      <c r="D6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="I1:K2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="E2:F2"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
attempt to correct pricing problem between ASHP and wood boiler
</commit_message>
<xml_diff>
--- a/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
+++ b/cea_energy_hub_optimizer/data/example_techDefinition.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangy\Documents\GitHub\energy_hub_optimizer_calliope\cea_energy_hub_optimizer\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB6F493-256E-49A6-A8A5-D45B4AA0164D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D04766-6AE6-4140-863D-28459E1BC1AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
+    <workbookView xWindow="2310" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{3D0A62A3-FD81-47EE-AB31-50A82C57680E}"/>
   </bookViews>
   <sheets>
     <sheet name="supply" sheetId="5" r:id="rId1"/>
@@ -886,7 +886,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-HSLU, 2024</t>
+HSLU, 2024, 5-20</t>
         </r>
       </text>
     </comment>
@@ -963,7 +963,248 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{0E42BBB0-E2D2-4B44-A8FB-B6C155C3EBB8}">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{4EDF9681-2558-4030-8F05-B671FF192C20}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+HSLU 2024, 20-200</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{4AA31669-13E6-4ED6-B100-2D318CD5DB4D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+carnot efficiency 52%
+reference point temperature 0degC</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{56417D6D-26F8-4E61-B08D-E23610F8B227}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+HSLU, 2024, 5-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{641049B0-A4A9-4070-BE17-D18C9F965D2B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+HSLU with no interception</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{F03E95D3-22AC-4F5A-A01A-E49103ED38DC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+16-20, Danish energy agency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{1C8E9C67-B822-495B-ABCD-A96AAE09F507}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+HSLU 2024, 20-200</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{716F29CA-954E-4786-A780-C94E461733D3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+HSLU, 2024, 5-20</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{09CB5F3B-6E04-4BCC-A37A-F3ABBAD7BD61}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+HSLU with no interception</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M12" authorId="0" shapeId="0" xr:uid="{0C0424B8-830D-41AF-9090-E6C9C5134069}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+16-20, Danish energy agency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{B5F66556-A024-41B4-9586-9E3C374E77B7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yiqiao Wang:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+HSLU 2024, 20-200</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="0" shapeId="0" xr:uid="{0E42BBB0-E2D2-4B44-A8FB-B6C155C3EBB8}">
       <text>
         <r>
           <rPr>
@@ -988,79 +1229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{46319015-5968-48C6-8727-6AE198B9B42F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-HSLU, 2024</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{641049B0-A4A9-4070-BE17-D18C9F965D2B}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-HSLU with no interception</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{F03E95D3-22AC-4F5A-A01A-E49103ED38DC}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-16-20, Danish energy agency</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{C5D0AF4C-BF2F-4C21-9650-2E8E580F6C8C}">
+    <comment ref="J15" authorId="0" shapeId="0" xr:uid="{C5D0AF4C-BF2F-4C21-9650-2E8E580F6C8C}">
       <text>
         <r>
           <rPr>
@@ -1084,79 +1253,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{9F9AE665-A739-45ED-ADA8-E7DA8074E02F}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-HSLU, 2024</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{09CB5F3B-6E04-4BCC-A37A-F3ABBAD7BD61}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-HSLU with no interception</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M12" authorId="0" shapeId="0" xr:uid="{0C0424B8-830D-41AF-9090-E6C9C5134069}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yiqiao Wang:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-16-20, Danish energy agency</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{D1B835A7-01F4-4396-B76E-4D0C73741027}">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{D1B835A7-01F4-4396-B76E-4D0C73741027}">
       <text>
         <r>
           <rPr>
@@ -1180,7 +1277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{AB00EA6B-EDC9-4CF5-B490-4899A5405AC4}">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{AB00EA6B-EDC9-4CF5-B490-4899A5405AC4}">
       <text>
         <r>
           <rPr>
@@ -1204,7 +1301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{32220E44-B3A9-4388-B223-558CBD5E3D40}">
+    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{32220E44-B3A9-4388-B223-558CBD5E3D40}">
       <text>
         <r>
           <rPr>
@@ -1228,7 +1325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{4A7C72F0-7DE0-4554-AF5C-D1918452E588}">
+    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{4A7C72F0-7DE0-4554-AF5C-D1918452E588}">
       <text>
         <r>
           <rPr>
@@ -1252,7 +1349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I18" authorId="0" shapeId="0" xr:uid="{8B7A05C7-D040-4169-AD2E-35122D0CCCDF}">
+    <comment ref="I21" authorId="0" shapeId="0" xr:uid="{8B7A05C7-D040-4169-AD2E-35122D0CCCDF}">
       <text>
         <r>
           <rPr>
@@ -1276,7 +1373,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{CB1A0D7B-E5FD-4735-8255-AA5171D239DF}">
+    <comment ref="H23" authorId="0" shapeId="0" xr:uid="{CB1A0D7B-E5FD-4735-8255-AA5171D239DF}">
       <text>
         <r>
           <rPr>
@@ -1300,7 +1397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I21" authorId="0" shapeId="0" xr:uid="{6FC2FE87-96A6-4E67-8D36-DD5F481FA6F9}">
+    <comment ref="I24" authorId="0" shapeId="0" xr:uid="{6FC2FE87-96A6-4E67-8D36-DD5F481FA6F9}">
       <text>
         <r>
           <rPr>
@@ -1324,7 +1421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M23" authorId="0" shapeId="0" xr:uid="{AF2745AD-0BD1-40F0-B7C8-39776BC84E0B}">
+    <comment ref="M26" authorId="0" shapeId="0" xr:uid="{AF2745AD-0BD1-40F0-B7C8-39776BC84E0B}">
       <text>
         <r>
           <rPr>
@@ -2047,7 +2144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="133">
   <si>
     <t>monetary</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2241,10 +2338,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ASHP_35</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GSHP_35</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2253,14 +2346,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ASHP_60</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ASHP_85</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>heat_65</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2532,14 +2617,7 @@
     <t>supply_for_pv</t>
   </si>
   <si>
-    <t>ASHP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GSHP</t>
-  </si>
-  <si>
-    <t>GSHP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2559,6 +2637,30 @@
   </si>
   <si>
     <t>district_heating_techs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASHP_35_small</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASHP_35_large</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASHP_60_small</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASHP_60_large</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASHP_85_small</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ASHP_85_large</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3029,15 +3131,15 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.35546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3076,10 +3178,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
@@ -3099,7 +3201,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -3122,7 +3224,7 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
         <v>32</v>
@@ -3145,7 +3247,7 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -3168,7 +3270,7 @@
         <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -3191,7 +3293,7 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -3226,22 +3328,22 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -3294,31 +3396,31 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>21</v>
@@ -3338,7 +3440,7 @@
         <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E4">
         <v>3000</v>
@@ -3355,10 +3457,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E5">
         <v>1600</v>
@@ -3375,10 +3477,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E6">
         <v>1300</v>
@@ -3392,13 +3494,13 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" t="s">
         <v>120</v>
-      </c>
-      <c r="B7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" t="s">
-        <v>123</v>
       </c>
       <c r="E7">
         <v>1000</v>
@@ -3412,16 +3514,16 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E8">
         <v>1576</v>
@@ -3433,13 +3535,13 @@
         <v>290</v>
       </c>
       <c r="H8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K8">
         <v>1.2969999999999999</v>
@@ -3453,13 +3555,13 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D9" t="s">
         <v>47</v>
@@ -3474,13 +3576,13 @@
         <v>296</v>
       </c>
       <c r="H9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="K9">
         <v>1.41</v>
@@ -3507,26 +3609,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A246388-C9BA-4771-92A8-398DB13C28C5}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7:Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -3577,13 +3679,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>14</v>
@@ -3615,7 +3717,7 @@
         <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F4">
         <v>371.80000000000013</v>
@@ -3635,7 +3737,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F5">
         <v>180.88</v>
@@ -3655,7 +3757,7 @@
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F6">
         <v>117.4</v>
@@ -3675,7 +3777,7 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F7">
         <v>72.010000000000005</v>
@@ -3692,332 +3794,519 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" t="s">
-        <v>124</v>
+        <v>84</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>49</v>
+      </c>
+      <c r="F8">
+        <v>1260</v>
+      </c>
+      <c r="G8">
+        <v>23800</v>
+      </c>
+      <c r="H8">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="I8">
+        <v>45.9</v>
       </c>
       <c r="J8">
         <v>4.58</v>
       </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>20</v>
+      </c>
+      <c r="M8">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E9" t="s">
-        <v>50</v>
+      <c r="F9">
+        <v>1843.33</v>
+      </c>
+      <c r="G9">
+        <v>12133.33</v>
+      </c>
+      <c r="H9">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="I9">
+        <v>45.9</v>
       </c>
       <c r="J9">
-        <v>7.64</v>
+        <v>4.58</v>
+      </c>
+      <c r="K9">
+        <v>20</v>
+      </c>
+      <c r="L9">
+        <v>200</v>
+      </c>
+      <c r="M9">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>129</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" t="s">
-        <v>124</v>
+        <v>84</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>1260</v>
+      </c>
+      <c r="G10">
+        <v>23800</v>
+      </c>
+      <c r="H10">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="I10">
+        <v>45.9</v>
       </c>
       <c r="J10">
         <v>2.89</v>
       </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>20</v>
+      </c>
+      <c r="M10">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="1"/>
+        <v>130</v>
+      </c>
       <c r="C11" t="s">
-        <v>125</v>
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="F11">
+        <v>1843.33</v>
+      </c>
+      <c r="G11">
+        <v>12133.33</v>
+      </c>
+      <c r="H11">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="I11">
+        <v>45.9</v>
       </c>
       <c r="J11">
-        <v>4.13</v>
+        <v>2.89</v>
+      </c>
+      <c r="K11">
+        <v>20</v>
+      </c>
+      <c r="L11">
+        <v>200</v>
+      </c>
+      <c r="M11">
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>131</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>124</v>
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
       </c>
       <c r="E12" t="s">
         <v>47</v>
       </c>
+      <c r="F12">
+        <v>1260</v>
+      </c>
+      <c r="G12">
+        <v>23800</v>
+      </c>
+      <c r="H12">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="I12">
+        <v>45.9</v>
+      </c>
       <c r="J12">
         <v>2.2000000000000002</v>
       </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>20</v>
+      </c>
+      <c r="M12">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>132</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>84</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
       </c>
       <c r="E13" t="s">
         <v>47</v>
       </c>
+      <c r="F13">
+        <v>1843.33</v>
+      </c>
+      <c r="G13">
+        <v>12133.33</v>
+      </c>
+      <c r="H13">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="I13">
+        <v>45.9</v>
+      </c>
       <c r="J13">
-        <v>2.96</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K13">
+        <v>20</v>
+      </c>
+      <c r="L13">
+        <v>200</v>
+      </c>
+      <c r="M13">
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>128</v>
-      </c>
-      <c r="F14">
-        <v>300</v>
-      </c>
-      <c r="G14">
-        <v>17200</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>20</v>
+        <v>121</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14">
+        <v>7.64</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="B15" s="1"/>
       <c r="C15" t="s">
-        <v>130</v>
-      </c>
-      <c r="F15">
-        <v>880</v>
-      </c>
-      <c r="G15">
-        <v>25100</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>20</v>
+        <v>121</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15">
+        <v>4.13</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>29</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B16" s="1"/>
       <c r="C16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F16">
-        <v>486.7</v>
-      </c>
-      <c r="G16">
-        <v>20466.7</v>
-      </c>
-      <c r="K16">
-        <v>1</v>
-      </c>
-      <c r="L16">
-        <v>20</v>
+        <v>121</v>
+      </c>
+      <c r="E16" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16">
+        <v>2.96</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F17">
-        <v>176.7</v>
+        <v>300</v>
       </c>
       <c r="G17">
-        <v>19666.7</v>
+        <v>17200</v>
       </c>
       <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
         <v>20</v>
-      </c>
-      <c r="L17">
-        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F18">
-        <v>414.99999999999989</v>
+        <v>880</v>
       </c>
       <c r="G18">
-        <v>34400.000000000015</v>
+        <v>25100</v>
       </c>
       <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
         <v>20</v>
-      </c>
-      <c r="L18">
-        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F19">
-        <v>189.4</v>
+        <v>486.7</v>
       </c>
       <c r="G19">
-        <v>26411.1</v>
+        <v>20466.7</v>
       </c>
       <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
         <v>20</v>
-      </c>
-      <c r="L19">
-        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F20">
-        <v>155.30000000000001</v>
+        <v>176.7</v>
       </c>
       <c r="G20">
-        <v>23933.3</v>
+        <v>19666.7</v>
       </c>
       <c r="K20">
+        <v>20</v>
+      </c>
+      <c r="L20">
         <v>200</v>
-      </c>
-      <c r="L20">
-        <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F21">
-        <v>278.00000000000006</v>
+        <v>414.99999999999989</v>
       </c>
       <c r="G21">
-        <v>61799.999999999985</v>
+        <v>34400.000000000015</v>
       </c>
       <c r="K21">
+        <v>20</v>
+      </c>
+      <c r="L21">
         <v>200</v>
-      </c>
-      <c r="L21">
-        <v>500</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F22">
-        <v>211.7</v>
+        <v>189.4</v>
       </c>
       <c r="G22">
-        <v>21966.7</v>
+        <v>26411.1</v>
       </c>
       <c r="K22">
+        <v>20</v>
+      </c>
+      <c r="L22">
         <v>200</v>
-      </c>
-      <c r="L22">
-        <v>500</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>76</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="B23" s="1"/>
       <c r="C23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" t="s">
-        <v>66</v>
-      </c>
-      <c r="J23">
-        <v>1</v>
-      </c>
-      <c r="M23">
-        <v>1</v>
+        <v>123</v>
+      </c>
+      <c r="F23">
+        <v>155.30000000000001</v>
+      </c>
+      <c r="G23">
+        <v>23933.3</v>
+      </c>
+      <c r="K23">
+        <v>200</v>
+      </c>
+      <c r="L23">
+        <v>500</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>44</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" t="s">
-        <v>66</v>
-      </c>
-      <c r="E24" t="s">
-        <v>50</v>
-      </c>
-      <c r="J24">
+        <v>125</v>
+      </c>
+      <c r="F24">
+        <v>278.00000000000006</v>
+      </c>
+      <c r="G24">
+        <v>61799.999999999985</v>
+      </c>
+      <c r="K24">
+        <v>200</v>
+      </c>
+      <c r="L24">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>124</v>
+      </c>
+      <c r="F25">
+        <v>211.7</v>
+      </c>
+      <c r="G25">
+        <v>21966.7</v>
+      </c>
+      <c r="K25">
+        <v>200</v>
+      </c>
+      <c r="L25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J26">
         <v>1</v>
       </c>
-      <c r="M24">
+      <c r="M26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" t="s">
+        <v>49</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="M27">
         <v>1</v>
       </c>
     </row>
@@ -4042,31 +4331,31 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.35546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.2109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" customWidth="1"/>
-    <col min="17" max="17" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.25" customWidth="1"/>
-    <col min="22" max="22" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.640625" customWidth="1"/>
+    <col min="17" max="17" width="10.2109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.2109375" customWidth="1"/>
+    <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24">
@@ -4139,34 +4428,34 @@
         <v>7</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="M3" s="8" t="s">
         <v>13</v>
@@ -4178,18 +4467,18 @@
         <v>14</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>20</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="S3" s="9"/>
       <c r="T3" s="9"/>
       <c r="U3" s="9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="V3" s="8" t="s">
         <v>21</v>
@@ -4220,11 +4509,11 @@
       <c r="P4" s="8"/>
       <c r="Q4" s="8"/>
       <c r="R4" s="9" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="S4" s="9"/>
       <c r="T4" s="6" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="U4" s="9"/>
       <c r="V4" s="8"/>
@@ -4250,10 +4539,10 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="T5" s="5" t="s">
         <v>31</v>
@@ -4265,22 +4554,22 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
         <v>32</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s">
         <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="J6">
         <v>1108.2</v>
@@ -4326,18 +4615,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="Q3:Q5"/>
-    <mergeCell ref="W3:W5"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="I3:I5"/>
-    <mergeCell ref="G3:G5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="L3:L5"/>
-    <mergeCell ref="U3:U5"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="D3:D5"/>
@@ -4354,6 +4631,18 @@
     <mergeCell ref="R3:T3"/>
     <mergeCell ref="X3:X5"/>
     <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="Q3:Q5"/>
+    <mergeCell ref="W3:W5"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="I3:I5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="L3:L5"/>
+    <mergeCell ref="U3:U5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4369,21 +4658,21 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="16.5" defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.35546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.4140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.08203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.08203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.08203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.0703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.0703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.0703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.2109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -4434,34 +4723,34 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>20</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>17</v>
@@ -4475,7 +4764,7 @@
         <v>27</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -4510,16 +4799,16 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H5">
         <v>0.96</v>
@@ -4530,16 +4819,16 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="H6">
         <v>0.95</v>
@@ -4550,13 +4839,13 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
         <v>47</v>
@@ -4589,13 +4878,13 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.15"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.35546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.2109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4624,115 +4913,115 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" t="s">
         <v>99</v>
       </c>
-      <c r="B4" t="s">
-        <v>102</v>
-      </c>
       <c r="C4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
         <v>103</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
         <v>106</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s">
         <v>106</v>
-      </c>
-      <c r="D6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
         <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" t="s">
         <v>104</v>
       </c>
-      <c r="C8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>107</v>
-      </c>
-      <c r="E8" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>